<commit_message>
Merged golem techs & closes #375
</commit_message>
<xml_diff>
--- a/Localizations/STRINGS_10.xlsx
+++ b/Localizations/STRINGS_10.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="343">
   <si>
     <t xml:space="preserve"># Language = English ; change this to the name of the language being localized to</t>
   </si>
@@ -1037,6 +1037,18 @@
   </si>
   <si>
     <t xml:space="preserve">Siege tactics are tactical plans for the construction and use of improvised battlefield fortifications. This increases the speed at which all companies entrench and fortify.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Golemancy ProperName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Golemancy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Golemancy Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The use of powerful elemental magic has imbued a semblance of life into the very earth, creating mindless warriors that feel no pain. Those wrought from khaldunite-bearing stone are particularly dangerous.</t>
   </si>
 </sst>
 </file>
@@ -1162,8 +1174,8 @@
   </sheetPr>
   <dimension ref="A1:H163"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A139" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H151" activeCellId="0" sqref="H151"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E139" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H153" activeCellId="0" sqref="H153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4700,7 +4712,7 @@
         <v>STRING_6155_The_Slaanri_Champions_are_the_strongest_and_deadliest_of_the_Slaanri_warriors__In_honor_of_their_powerful_and_violent_cousins__they_wield_forked_bone_spears_in_combat__They_have_taught_the_construction_technique_of_these_fearsome_weapons__allowing_for_the_creation_of_more_effective_arms_for_spear_wielding_troops_</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="1" t="n">
         <f aca="false">A149+1</f>
         <v>6156</v>
@@ -4720,7 +4732,7 @@
         <v>Siege Tactics</v>
       </c>
       <c r="G150" s="0" t="s">
-        <v>283</v>
+        <v>299</v>
       </c>
       <c r="H150" s="1" t="str">
         <f aca="false">"STRING_"&amp;A150&amp;"_"&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($D150," ","_"),",","_"),".","_"),"'","_"),"-","_"),"%","_"),"+","_")</f>
@@ -4754,42 +4766,58 @@
         <v>STRING_6157_Siege_tactics_are_tactical_plans_for_the_construction_and_use_of_improvised_battlefield_fortifications__This_increases_the_speed_at_which_all_companies_entrench_and_fortify_</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="1" t="n">
         <f aca="false">A151+1</f>
         <v>6158</v>
       </c>
-      <c r="B152" s="1"/>
+      <c r="B152" s="1" t="s">
+        <v>339</v>
+      </c>
       <c r="C152" s="1" t="n">
         <f aca="false">LEN(D152)</f>
-        <v>0</v>
-      </c>
-      <c r="E152" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E152" s="1" t="str">
         <f aca="false">D152</f>
-        <v>0</v>
+        <v>Golemancy</v>
+      </c>
+      <c r="G152" s="0" t="s">
+        <v>299</v>
       </c>
       <c r="H152" s="1" t="str">
         <f aca="false">"STRING_"&amp;A152&amp;"_"&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($D152," ","_"),",","_"),".","_"),"'","_"),"-","_"),"%","_"),"+","_")</f>
-        <v>STRING_6158_</v>
-      </c>
-    </row>
-    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>STRING_6158_Golemancy</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="39.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="1" t="n">
         <f aca="false">A152+1</f>
         <v>6159</v>
       </c>
-      <c r="B153" s="1"/>
+      <c r="B153" s="1" t="s">
+        <v>341</v>
+      </c>
       <c r="C153" s="1" t="n">
         <f aca="false">LEN(D153)</f>
-        <v>0</v>
-      </c>
-      <c r="E153" s="1" t="n">
+        <v>205</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="E153" s="1" t="str">
         <f aca="false">D153</f>
-        <v>0</v>
+        <v>The use of powerful elemental magic has imbued a semblance of life into the very earth, creating mindless warriors that feel no pain. Those wrought from khaldunite-bearing stone are particularly dangerous.</v>
+      </c>
+      <c r="G153" s="0" t="s">
+        <v>283</v>
       </c>
       <c r="H153" s="1" t="str">
         <f aca="false">"STRING_"&amp;A153&amp;"_"&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($D153," ","_"),",","_"),".","_"),"'","_"),"-","_"),"%","_"),"+","_")</f>
-        <v>STRING_6159_</v>
+        <v>STRING_6159_The_use_of_powerful_elemental_magic_has_imbued_a_semblance_of_life_into_the_very_earth__creating_mindless_warriors_that_feel_no_pain__Those_wrought_from_khaldunite_bearing_stone_are_particularly_dangerous_</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Combined Conjuror & Summoning Scrolls & closes #379
</commit_message>
<xml_diff>
--- a/Localizations/STRINGS_10.xlsx
+++ b/Localizations/STRINGS_10.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="347">
   <si>
     <t xml:space="preserve"># Language = English ; change this to the name of the language being localized to</t>
   </si>
@@ -1049,6 +1049,18 @@
   </si>
   <si>
     <t xml:space="preserve">The use of powerful elemental magic has imbued a semblance of life into the very earth, creating mindless warriors that feel no pain. Those wrought from khaldunite-bearing stone are particularly dangerous.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conjurors' Academy ProperName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conjurors' Academy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conjurors' Academy Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your kingdom's mages have delved into the dark side of summoning, and these fearsome Conjurors have learned the secret of calling forth creatures of Shadow. Their arcane research has led to new techniques that produce stronger and healthier mystical beasts; All summoned creatures have more health and deal more damage than normal.</t>
   </si>
 </sst>
 </file>
@@ -1174,8 +1186,8 @@
   </sheetPr>
   <dimension ref="A1:H163"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E139" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H153" activeCellId="0" sqref="H153"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A142" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G154" activeCellId="0" sqref="G154:G155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4820,42 +4832,58 @@
         <v>STRING_6159_The_use_of_powerful_elemental_magic_has_imbued_a_semblance_of_life_into_the_very_earth__creating_mindless_warriors_that_feel_no_pain__Those_wrought_from_khaldunite_bearing_stone_are_particularly_dangerous_</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="1" t="n">
         <f aca="false">A153+1</f>
         <v>6160</v>
       </c>
-      <c r="B154" s="1"/>
+      <c r="B154" s="5" t="s">
+        <v>343</v>
+      </c>
       <c r="C154" s="1" t="n">
         <f aca="false">LEN(D154)</f>
-        <v>0</v>
-      </c>
-      <c r="E154" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="D154" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="E154" s="1" t="str">
         <f aca="false">D154</f>
-        <v>0</v>
+        <v>Conjurors' Academy</v>
+      </c>
+      <c r="G154" s="0" t="s">
+        <v>299</v>
       </c>
       <c r="H154" s="1" t="str">
         <f aca="false">"STRING_"&amp;A154&amp;"_"&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($D154," ","_"),",","_"),".","_"),"'","_"),"-","_"),"%","_"),"+","_")</f>
-        <v>STRING_6160_</v>
-      </c>
-    </row>
-    <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>STRING_6160_Conjurors__Academy</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="51.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="1" t="n">
         <f aca="false">A154+1</f>
         <v>6161</v>
       </c>
-      <c r="B155" s="1"/>
+      <c r="B155" s="5" t="s">
+        <v>345</v>
+      </c>
       <c r="C155" s="1" t="n">
         <f aca="false">LEN(D155)</f>
-        <v>0</v>
-      </c>
-      <c r="E155" s="1" t="n">
+        <v>331</v>
+      </c>
+      <c r="D155" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="E155" s="1" t="str">
         <f aca="false">D155</f>
-        <v>0</v>
+        <v>Your kingdom's mages have delved into the dark side of summoning, and these fearsome Conjurors have learned the secret of calling forth creatures of Shadow. Their arcane research has led to new techniques that produce stronger and healthier mystical beasts; All summoned creatures have more health and deal more damage than normal.</v>
+      </c>
+      <c r="G155" s="0" t="s">
+        <v>283</v>
       </c>
       <c r="H155" s="1" t="str">
         <f aca="false">"STRING_"&amp;A155&amp;"_"&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($D155," ","_"),",","_"),".","_"),"'","_"),"-","_"),"%","_"),"+","_")</f>
-        <v>STRING_6161_</v>
+        <v>STRING_6161_Your_kingdom_s_mages_have_delved_into_the_dark_side_of_summoning__and_these_fearsome_Conjurors_have_learned_the_secret_of_calling_forth_creatures_of_Shadow__Their_arcane_research_has_led_to_new_techniques_that_produce_stronger_and_healthier_mystical_beasts;_All_summoned_creatures_have_more_health_and_deal_more_damage_than_normal_</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Combined Journeymen & Pioneer & closes #378
</commit_message>
<xml_diff>
--- a/Localizations/STRINGS_10.xlsx
+++ b/Localizations/STRINGS_10.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="353">
   <si>
     <t xml:space="preserve"># Language = English ; change this to the name of the language being localized to</t>
   </si>
@@ -1061,6 +1061,24 @@
   </si>
   <si>
     <t xml:space="preserve">Your kingdom's mages have delved into the dark side of summoning, and these fearsome Conjurors have learned the secret of calling forth creatures of Shadow. Their arcane research has led to new techniques that produce stronger and healthier mystical beasts; All summoned creatures have more health and deal more damage than normal.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Journeymen Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Journeymen's Guild is a special organization of laborers that train craftsmen and masons. Having their guild in your kingdom reduces the costs of constructing new building components and provides highly skilled workers for the construction of new settlements. Journeymen can be recruited in any Mareten settlement.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Journeyman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PIONEER.INI ProperName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Journeymen are expert craftsmen and builders. They can construct new settlements 50% faster than the less well-trained Settlers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PIONEER.INI Description</t>
   </si>
 </sst>
 </file>
@@ -1186,8 +1204,8 @@
   </sheetPr>
   <dimension ref="A1:H163"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A142" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G154" activeCellId="0" sqref="G154:G155"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E148" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H158" activeCellId="0" sqref="H158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4886,61 +4904,85 @@
         <v>STRING_6161_Your_kingdom_s_mages_have_delved_into_the_dark_side_of_summoning__and_these_fearsome_Conjurors_have_learned_the_secret_of_calling_forth_creatures_of_Shadow__Their_arcane_research_has_led_to_new_techniques_that_produce_stronger_and_healthier_mystical_beasts;_All_summoned_creatures_have_more_health_and_deal_more_damage_than_normal_</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="51.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="1" t="n">
         <f aca="false">A155+1</f>
         <v>6162</v>
       </c>
-      <c r="B156" s="1"/>
+      <c r="B156" s="1" t="s">
+        <v>347</v>
+      </c>
       <c r="C156" s="1" t="n">
         <f aca="false">LEN(D156)</f>
-        <v>0</v>
-      </c>
-      <c r="E156" s="1" t="n">
+        <v>318</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="E156" s="1" t="str">
         <f aca="false">D156</f>
-        <v>0</v>
+        <v>The Journeymen's Guild is a special organization of laborers that train craftsmen and masons. Having their guild in your kingdom reduces the costs of constructing new building components and provides highly skilled workers for the construction of new settlements. Journeymen can be recruited in any Mareten settlement.</v>
+      </c>
+      <c r="G156" s="0" t="s">
+        <v>283</v>
       </c>
       <c r="H156" s="1" t="str">
         <f aca="false">"STRING_"&amp;A156&amp;"_"&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($D156," ","_"),",","_"),".","_"),"'","_"),"-","_"),"%","_"),"+","_")</f>
-        <v>STRING_6162_</v>
-      </c>
-    </row>
-    <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>STRING_6162_The_Journeymen_s_Guild_is_a_special_organization_of_laborers_that_train_craftsmen_and_masons__Having_their_guild_in_your_kingdom_reduces_the_costs_of_constructing_new_building_components_and_provides_highly_skilled_workers_for_the_construction_of_new_settlements__Journeymen_can_be_recruited_in_any_Mareten_settlement_</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="1" t="n">
         <f aca="false">A156+1</f>
         <v>6163</v>
       </c>
-      <c r="B157" s="1"/>
+      <c r="B157" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="C157" s="1" t="n">
         <f aca="false">LEN(D157)</f>
-        <v>0</v>
-      </c>
-      <c r="E157" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="E157" s="1" t="str">
         <f aca="false">D157</f>
-        <v>0</v>
+        <v>Journeyman</v>
+      </c>
+      <c r="G157" s="0" t="s">
+        <v>350</v>
       </c>
       <c r="H157" s="1" t="str">
         <f aca="false">"STRING_"&amp;A157&amp;"_"&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($D157," ","_"),",","_"),".","_"),"'","_"),"-","_"),"%","_"),"+","_")</f>
-        <v>STRING_6163_</v>
-      </c>
-    </row>
-    <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>STRING_6163_Journeyman</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="1" t="n">
         <f aca="false">A157+1</f>
         <v>6164</v>
       </c>
-      <c r="B158" s="1"/>
+      <c r="B158" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="C158" s="1" t="n">
         <f aca="false">LEN(D158)</f>
-        <v>0</v>
-      </c>
-      <c r="E158" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="E158" s="1" t="str">
         <f aca="false">D158</f>
-        <v>0</v>
+        <v>Journeymen are expert craftsmen and builders. They can construct new settlements 50% faster than the less well-trained Settlers.</v>
+      </c>
+      <c r="G158" s="0" t="s">
+        <v>352</v>
       </c>
       <c r="H158" s="1" t="str">
         <f aca="false">"STRING_"&amp;A158&amp;"_"&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($D158," ","_"),",","_"),".","_"),"'","_"),"-","_"),"%","_"),"+","_")</f>
-        <v>STRING_6164_</v>
+        <v>STRING_6164_Journeymen_are_expert_craftsmen_and_builders__They_can_construct_new_settlements_50__faster_than_the_less_well_trained_Settlers_</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Exported STRINGS_10.xlsx to INI
</commit_message>
<xml_diff>
--- a/Localizations/STRINGS_10.xlsx
+++ b/Localizations/STRINGS_10.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="STRINGS_10" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Copysheet" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="368">
   <si>
     <t xml:space="preserve"># Language = English ; change this to the name of the language being localized to</t>
   </si>
@@ -1118,14 +1119,21 @@
   </si>
   <si>
     <t xml:space="preserve">Specially crafted spider-silk tunics that are light as air and can be worn under robes that can avert a stray arrow or similar missile with ease.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silken Robe Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robes woven from the silk of giant spiders, making them lighter and more resistant than the normal mage and priest robes.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -1199,7 +1207,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1228,6 +1236,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1245,10 +1257,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H175"/>
+  <dimension ref="A1:H240"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A150" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D165" activeCellId="0" sqref="D165"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A157" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5217,23 +5229,31 @@
         <v>STRING_6171_Specially_crafted_spider_silk_tunics_that_are_light_as_air_and_can_be_worn_under_robes_that_can_avert_a_stray_arrow_or_similar_missile_with_ease_</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="2" t="n">
         <f aca="false">A165+1</f>
         <v>6172</v>
       </c>
-      <c r="B166" s="2"/>
+      <c r="B166" s="2" t="s">
+        <v>366</v>
+      </c>
       <c r="C166" s="2" t="n">
         <f aca="false">LEN(D166)</f>
-        <v>0</v>
-      </c>
-      <c r="E166" s="2" t="n">
+        <v>121</v>
+      </c>
+      <c r="D166" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="E166" s="2" t="str">
         <f aca="false">D166</f>
-        <v>0</v>
+        <v>Robes woven from the silk of giant spiders, making them lighter and more resistant than the normal mage and priest robes.</v>
+      </c>
+      <c r="G166" s="1" t="s">
+        <v>283</v>
       </c>
       <c r="H166" s="2" t="str">
         <f aca="false">"STRING_"&amp;A166&amp;"_"&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($D166," ","_"),",","_"),".","_"),"'","_"),"-","_"),"%","_"),"+","_")</f>
-        <v>STRING_6172_</v>
+        <v>STRING_6172_Robes_woven_from_the_silk_of_giant_spiders__making_them_lighter_and_more_resistant_than_the_normal_mage_and_priest_robes_</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5407,6 +5427,56 @@
         <v>STRING_6181_</v>
       </c>
     </row>
+    <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -5416,4 +5486,4037 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F200"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A164" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E187" activeCellId="0" sqref="E187"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.8046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="27.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="51.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="28.44"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="str">
+        <f aca="false" t="array" ref="A1:D200">STRINGS_10!A1:D200</f>
+        <v># Language = English ; change this to the name of the language being localized to</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <f aca="false" t="array" ref="E1:E200">STRINGS_10!E1:E200</f>
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <f aca="false" t="array" ref="F1:F200">STRINGS_10!G1:G200</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="str">
+        <v>#</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="str">
+        <v># This file contains all new text for Kohan Gold to allow for localization into other languages</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="str">
+        <v># To add a new language, create a new &lt;Localized Text (lang_code)&gt; column, then add translations of the text in the &lt;Source Text&gt; column</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="str">
+        <v>#</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="str">
+        <v># Do not insert any other new columns</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="str">
+        <v># </v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="str">
+        <v># Any text may be added to &lt;Comment&gt; column, this is used only for the translator's notes, will not be visible in game</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="str">
+        <v># </v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="str">
+        <v># Save intermediate changes in Excel format, but final Strings_10.ini file must be in tab-delimited format</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="str">
+        <v># When saving to tab delimited format, first make a copy of this spreadsheet and delete all &lt;Localized Text&gt; columns but the desired one, as well as the &lt;INI Text&gt; column.</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="str">
+        <v># Rename the remaining translation column to &lt;Localized Text&gt; (that is, remove the  (lang_code) from the name), then use Ctrl+A Ctrl+C to copy the whole sheet and paste it into a blank .INI file</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="str">
+        <v># Make sure the .INI file is set to to the ANSI character set, and convert to it if needed</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="str">
+        <v># </v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="str">
+        <v># New rows may be inserted, but only for comment purposes, any rows starting with '#' will be ignored as comments</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="str">
+        <v># </v>
+      </c>
+      <c r="B16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="str">
+        <v># STRINGS_09 ends with ID 6032, so this file should start at ID 6033</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="str">
+        <v># String ID</v>
+      </c>
+      <c r="B18" s="1" t="str">
+        <v>Type</v>
+      </c>
+      <c r="C18" s="1" t="str">
+        <v>Constraints</v>
+      </c>
+      <c r="D18" s="1" t="str">
+        <v>Source Text</v>
+      </c>
+      <c r="E18" s="1" t="str">
+        <v>Localized Text (EN)</v>
+      </c>
+      <c r="F18" s="1" t="str">
+        <v>Comment</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="str">
+        <v># Heroes ==============================</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="n">
+        <v>6033</v>
+      </c>
+      <c r="B20" s="1" t="str">
+        <v>UnitData Description</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>530</v>
+      </c>
+      <c r="D20" s="1" t="str">
+        <v>A crack shot with the bow and equally deadly with his sword, Aethan Farhyd is one of the Nationalists' fiercest warriors. Always dressed in black from head to toe, Aethan prefers to keep to himself, usually skulking in the shadows. If he is found with others, it is usually with his close companions and only friends, Sebastian Atafeh and Ahikar Iraj. If those two are found together, he is often not far behind. It has long been rumored that Aethan had feelings for Ahikar, but if that is true, he has kept those feelings hidden.</v>
+      </c>
+      <c r="E20" s="1" t="str">
+        <v>A crack shot with the bow and equally deadly with his sword, Aethan Farhyd is one of the Nationalists' fiercest warriors. Always dressed in black from head to toe, Aethan prefers to keep to himself, usually skulking in the shadows. If he is found with others, it is usually with his close companions and only friends, Sebastian Atafeh and Ahikar Iraj. If those two are found together, he is often not far behind. It has long been rumored that Aethan had feelings for Ahikar, but if that is true, he has kept those feelings hidden.</v>
+      </c>
+      <c r="F20" s="1" t="str">
+        <v>Aethan Farhyd Description</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="n">
+        <v>6034</v>
+      </c>
+      <c r="B21" s="1" t="str">
+        <v>UnitData Description</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>539</v>
+      </c>
+      <c r="D21" s="1" t="str">
+        <v>Beloved wife of Sebastian Atafeh, the comely Ahikar Iraj is a fierce warrior in her own right. Ahikar wields a bow named Del'Kostan that gets more accurate the more she uses it in battle. Ahikar is the last living member of the House Iraj, once one of the most powerful Houses in the Council. Ahikar turned from the Council and joined the Nationalist movement when her House was slain and their amulets captured by the treacherous Ceyah Kohan, Ma'ar Nasai. She has sworn vengeance against the Ceyah at any cost by whatever means necessary.</v>
+      </c>
+      <c r="E21" s="1" t="str">
+        <v>Beloved wife of Sebastian Atafeh, the comely Ahikar Iraj is a fierce warrior in her own right. Ahikar wields a bow named Del'Kostan that gets more accurate the more she uses it in battle. Ahikar is the last living member of the House Iraj, once one of the most powerful Houses in the Council. Ahikar turned from the Council and joined the Nationalist movement when her House was slain and their amulets captured by the treacherous Ceyah Kohan, Ma'ar Nasai. She has sworn vengeance against the Ceyah at any cost by whatever means necessary.</v>
+      </c>
+      <c r="F21" s="1" t="str">
+        <v>Ahikar Iraj Description</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="n">
+        <v>6035</v>
+      </c>
+      <c r="B22" s="1" t="str">
+        <v>UnitData Description</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>395</v>
+      </c>
+      <c r="D22" s="1" t="str">
+        <v>A tall, athletic woman, Dali Azade is legendary for her speed and strength. She can outrun a horse over any distance and she never tires. She is disdainful of those who charge into battle on horseback, believing that a true warrior would face death on foot. Dali practices a form of meditation and control over her mind and body that renders her immune to enchantment and the effects of fatigue.</v>
+      </c>
+      <c r="E22" s="1" t="str">
+        <v>A tall, athletic woman, Dali Azade is legendary for her speed and strength. She can outrun a horse over any distance and she never tires. She is disdainful of those who charge into battle on horseback, believing that a true warrior would face death on foot. Dali practices a form of meditation and control over her mind and body that renders her immune to enchantment and the effects of fatigue.</v>
+      </c>
+      <c r="F22" s="1" t="str">
+        <v>Dali Azade Description</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="n">
+        <v>6036</v>
+      </c>
+      <c r="B23" s="1" t="str">
+        <v>UnitData Description</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>561</v>
+      </c>
+      <c r="D23" s="1" t="str">
+        <v>Darya Azar is dedicated to two things in life, the eradication of the Ceyah and the Royalist cause. Because the two are often inextricably intertwined, she is single-minded in her focus, choosing to ignore everything else in her life. While attractive, her hair is often unkempt and her eyes often have the glint of a zealot on a mission. All her actions are filled with an unshakable fervor and belief in her goal. She will do anything to accomplish her task, and only her devotion to the Royalist cause has kept her from being lumped in with the Nationalists.</v>
+      </c>
+      <c r="E23" s="1" t="str">
+        <v>Darya Azar is dedicated to two things in life, the eradication of the Ceyah and the Royalist cause. Because the two are often inextricably intertwined, she is single-minded in her focus, choosing to ignore everything else in her life. While attractive, her hair is often unkempt and her eyes often have the glint of a zealot on a mission. All her actions are filled with an unshakable fervor and belief in her goal. She will do anything to accomplish her task, and only her devotion to the Royalist cause has kept her from being lumped in with the Nationalists.</v>
+      </c>
+      <c r="F23" s="1" t="str">
+        <v>Darya Azar Description</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="n">
+        <v>6037</v>
+      </c>
+      <c r="B24" s="1" t="str">
+        <v>UnitData Description</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>513</v>
+      </c>
+      <c r="D24" s="1" t="str">
+        <v>Never far from Amon Koth, Jhaengus serves as lieutenant and advisor to the progenitor of the Rhaksha. As a warrior, Jhaengus is ferocious and almost unstoppable, but as an advisor, his feral nature renders most of his advice unpalatable even to Amon Koth. No one outside of Amon Koth knows the true nature of Jhaengus, or who he was before his transformation into this hideous beast of carnage and death. One thing is known for sure, his loyalty to Amon Koth is unquestionable and his lust for blood unquenchable.</v>
+      </c>
+      <c r="E24" s="1" t="str">
+        <v>Never far from Amon Koth, Jhaengus serves as lieutenant and advisor to the progenitor of the Rhaksha. As a warrior, Jhaengus is ferocious and almost unstoppable, but as an advisor, his feral nature renders most of his advice unpalatable even to Amon Koth. No one outside of Amon Koth knows the true nature of Jhaengus, or who he was before his transformation into this hideous beast of carnage and death. One thing is known for sure, his loyalty to Amon Koth is unquestionable and his lust for blood unquenchable.</v>
+      </c>
+      <c r="F24" s="1" t="str">
+        <v>Jhaengus Description</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="n">
+        <v>6038</v>
+      </c>
+      <c r="B25" s="1" t="str">
+        <v>UnitData Description</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>511</v>
+      </c>
+      <c r="D25" s="1" t="str">
+        <v>As beautiful as she is deadly, Jilla Jannat thrives on conflict and debate and always seems to emerge victorious. Her raven black hair and sea-green eyes are at odds with the grim set of her lips and her aquiline nose. She eschewed the Nationalist leanings of her House and followed the path of the Council. Outwardly her actions have all supported the Council, though she has been accused of being sympathetic to the Ceyah. Outside of Council meetings Jilla keeps to herself, preferring to work in the shadows.</v>
+      </c>
+      <c r="E25" s="1" t="str">
+        <v>As beautiful as she is deadly, Jilla Jannat thrives on conflict and debate and always seems to emerge victorious. Her raven black hair and sea-green eyes are at odds with the grim set of her lips and her aquiline nose. She eschewed the Nationalist leanings of her House and followed the path of the Council. Outwardly her actions have all supported the Council, though she has been accused of being sympathetic to the Ceyah. Outside of Council meetings Jilla keeps to herself, preferring to work in the shadows.</v>
+      </c>
+      <c r="F25" s="1" t="str">
+        <v>Jilla Jannat Description</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="n">
+        <v>6039</v>
+      </c>
+      <c r="B26" s="1" t="str">
+        <v>UnitData Description</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <v>638</v>
+      </c>
+      <c r="D26" s="1" t="str">
+        <v>His confidants know that when Lucius commits himself to something, he considers it an irrevocable pledge to give everything he can to make it happen. It is this trait that makes him a staunch ally and an implacable foe.  A angry scar cutting across his face, haunted sky-blue eyes, and grim nature conceal a man who was once handsome, jovial, and a leading member of the Council. Lucius broke from the rest of House Ajam and joined the Royalist cause in the Sixth Age when his wife Lydian was killed and her amulet captured by the Ceyah. He became a tireless and bitter foe of the Ceyah, and to this day he searches for his wife's amulet.</v>
+      </c>
+      <c r="E26" s="1" t="str">
+        <v>His confidants know that when Lucius commits himself to something, he considers it an irrevocable pledge to give everything he can to make it happen. It is this trait that makes him a staunch ally and an implacable foe.  A angry scar cutting across his face, haunted sky-blue eyes, and grim nature conceal a man who was once handsome, jovial, and a leading member of the Council. Lucius broke from the rest of House Ajam and joined the Royalist cause in the Sixth Age when his wife Lydian was killed and her amulet captured by the Ceyah. He became a tireless and bitter foe of the Ceyah, and to this day he searches for his wife's amulet.</v>
+      </c>
+      <c r="F26" s="1" t="str">
+        <v>Lucius Ajam Description</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="n">
+        <v>6040</v>
+      </c>
+      <c r="B27" s="1" t="str">
+        <v>UnitData Description</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <v>544</v>
+      </c>
+      <c r="D27" s="1" t="str">
+        <v>Mausallas Bahram possesses an unusual beauty, her unkempt shock of reddish-blonde hair and prominent nose conflicting with her serene brown eyes and ruby-red lips. Her beauty belies her intense intelligence and commanding grasp of the realm of magic. She is an accomplished warrior-mage, often found leading the charge against the forces of the Shadow, as well as wreaking havoc with her command of lightning. In melee, Mausallas wields a blackened longsword called Sta'archan that slices through the armor of her enemies with frightening ease.</v>
+      </c>
+      <c r="E27" s="1" t="str">
+        <v>Mausallas Bahram possesses an unusual beauty, her unkempt shock of reddish-blonde hair and prominent nose conflicting with her serene brown eyes and ruby-red lips. Her beauty belies her intense intelligence and commanding grasp of the realm of magic. She is an accomplished warrior-mage, often found leading the charge against the forces of the Shadow, as well as wreaking havoc with her command of lightning. In melee, Mausallas wields a blackened longsword called Sta'archan that slices through the armor of her enemies with frightening ease.</v>
+      </c>
+      <c r="F27" s="1" t="str">
+        <v>Mausallas Bahram Description</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="n">
+        <v>6041</v>
+      </c>
+      <c r="B28" s="1" t="str">
+        <v>UnitData Description</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>808</v>
+      </c>
+      <c r="D28" s="1" t="str">
+        <v>A giant of a man, Sebastian Atafeh is a formidable opponent on the battlefield. Caring little for caution and planning, Sebastian runs headlong into life assuming that he'll be able to fight his way out of whatever problems he encounters. While not a traditional leader, Sebastian often inspires others to great feats of courage and physical strength. His flowing hair, bushy beard, and refusal to wear any sort of helmet, mark him on the battlefield for all to see. Sebastian's devotion to the Nationalist cause is outmatched only by his devotion to his wife Ahikar. It is said that when she tasted her first death, he fought through hundreds of vile beasts of the Shadow to reach her amulet before it could be spirited away. Now, he is rarely far from her side, having never forgiven himself for her death.</v>
+      </c>
+      <c r="E28" s="1" t="str">
+        <v>A giant of a man, Sebastian Atafeh is a formidable opponent on the battlefield. Caring little for caution and planning, Sebastian runs headlong into life assuming that he'll be able to fight his way out of whatever problems he encounters. While not a traditional leader, Sebastian often inspires others to great feats of courage and physical strength. His flowing hair, bushy beard, and refusal to wear any sort of helmet, mark him on the battlefield for all to see. Sebastian's devotion to the Nationalist cause is outmatched only by his devotion to his wife Ahikar. It is said that when she tasted her first death, he fought through hundreds of vile beasts of the Shadow to reach her amulet before it could be spirited away. Now, he is rarely far from her side, having never forgiven himself for her death.</v>
+      </c>
+      <c r="F28" s="1" t="str">
+        <v>Sebastian Atafeh Description</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="n">
+        <v>6042</v>
+      </c>
+      <c r="B29" s="1" t="str">
+        <v>UnitData Description</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>828</v>
+      </c>
+      <c r="D29" s="1" t="str">
+        <v>One of the greatest generals in the history of the Council, Solomon Ghaffar once served as Darius Javidan's right-hand man and his military prowess is legendary. When Darius's death precipitated the Great Cataclysm, Solomon was the first to mobilize the military for the fight against the Ceyah. His youthful appearance belies his almost encyclopedic knowledge of military tactics and strategy. It was Solomon who led the search for the treacherous Vashti, and it was Solomon who led the armies of the Council against the Ceyah throughout the Second Age. He was slain by the bow of Melchior late in the Second Age, but his amulet was spirited away and he was reawakened almost immediately. He has been a tireless warrior since, tasting defeat only rarely, and influencing generations of Mareten with his leadership and chivalry.</v>
+      </c>
+      <c r="E29" s="1" t="str">
+        <v>One of the greatest generals in the history of the Council, Solomon Ghaffar once served as Darius Javidan's right-hand man and his military prowess is legendary. When Darius's death precipitated the Great Cataclysm, Solomon was the first to mobilize the military for the fight against the Ceyah. His youthful appearance belies his almost encyclopedic knowledge of military tactics and strategy. It was Solomon who led the search for the treacherous Vashti, and it was Solomon who led the armies of the Council against the Ceyah throughout the Second Age. He was slain by the bow of Melchior late in the Second Age, but his amulet was spirited away and he was reawakened almost immediately. He has been a tireless warrior since, tasting defeat only rarely, and influencing generations of Mareten with his leadership and chivalry.</v>
+      </c>
+      <c r="F29" s="1" t="str">
+        <v>Solomon Ghaffar Description</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="n">
+        <v>6043</v>
+      </c>
+      <c r="B30" s="1" t="str">
+        <v>UnitData Description</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <v>817</v>
+      </c>
+      <c r="D30" s="1" t="str">
+        <v>Zerin is an enigmatic figure, solitary and aloof even by the standards of the Kohan. Those that know him understand his grim nature for what it is - an obsession with uncovering the secrets of the cataclysms that have ravaged Khaldun. Once an avid scholar and prominent member of House Mordecai during the First Age, Zerin has since isolated himself from even his own House and focused solely on his research. Many speculate his research was responsible for the introduction of the Nightbringer to Nationalist society, though his fierce loyalty to the Nationalist cause is the only thing that is known for certain. In battle, Zerin is known for his ceremonial, heavily ornamented garbs and fearsome command of shadow magic. His ability to weaponise his dark knowledge has unnerved even the most powerful of the Ceyah.</v>
+      </c>
+      <c r="E30" s="1" t="str">
+        <v>Zerin is an enigmatic figure, solitary and aloof even by the standards of the Kohan. Those that know him understand his grim nature for what it is - an obsession with uncovering the secrets of the cataclysms that have ravaged Khaldun. Once an avid scholar and prominent member of House Mordecai during the First Age, Zerin has since isolated himself from even his own House and focused solely on his research. Many speculate his research was responsible for the introduction of the Nightbringer to Nationalist society, though his fierce loyalty to the Nationalist cause is the only thing that is known for certain. In battle, Zerin is known for his ceremonial, heavily ornamented garbs and fearsome command of shadow magic. His ability to weaponise his dark knowledge has unnerved even the most powerful of the Ceyah.</v>
+      </c>
+      <c r="F30" s="1" t="str">
+        <v>Zerin Mordecai Description</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="str">
+        <v># Units ==============================</v>
+      </c>
+      <c r="B31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="n">
+        <v>6044</v>
+      </c>
+      <c r="B32" s="1" t="str">
+        <v>ObjectData ProperName</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="D32" s="1" t="str">
+        <v>Phage Spider</v>
+      </c>
+      <c r="E32" s="1" t="str">
+        <v>Phage Spider</v>
+      </c>
+      <c r="F32" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="n">
+        <v>6045</v>
+      </c>
+      <c r="B33" s="1" t="str">
+        <v>ObjectData MonsterCompanyName</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="D33" s="1" t="str">
+        <v>Phage Spiders</v>
+      </c>
+      <c r="E33" s="1" t="str">
+        <v>Phage Spiders</v>
+      </c>
+      <c r="F33" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="n">
+        <v>6046</v>
+      </c>
+      <c r="B34" s="1" t="str">
+        <v>ObjectData ProperName</v>
+      </c>
+      <c r="C34" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="D34" s="1" t="str">
+        <v>Magma Elemental</v>
+      </c>
+      <c r="E34" s="1" t="str">
+        <v>Magma Elemental</v>
+      </c>
+      <c r="F34" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="n">
+        <v>6047</v>
+      </c>
+      <c r="B35" s="1" t="str">
+        <v>ObjectData MonsterCompanyName</v>
+      </c>
+      <c r="C35" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="D35" s="1" t="str">
+        <v>Magma Elementals</v>
+      </c>
+      <c r="E35" s="1" t="str">
+        <v>Magma Elementals</v>
+      </c>
+      <c r="F35" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="n">
+        <v>6048</v>
+      </c>
+      <c r="B36" s="1" t="str">
+        <v>UnitData Description</v>
+      </c>
+      <c r="C36" s="1" t="n">
+        <v>161</v>
+      </c>
+      <c r="D36" s="1" t="str">
+        <v>Magma Elementals are powerful creatures born from rock and fire. They let loose pyroclastic flows to scorch and suffocate anyone foolish enough to get too close.</v>
+      </c>
+      <c r="E36" s="1" t="str">
+        <v>Magma Elementals are powerful creatures born from rock and fire. They let loose pyroclastic flows to scorch and suffocate anyone foolish enough to get too close.</v>
+      </c>
+      <c r="F36" s="1" t="str">
+        <v>Cyrus Summon Description</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="n">
+        <v>6049</v>
+      </c>
+      <c r="B37" s="1" t="str">
+        <v>ObjectData ProperName</v>
+      </c>
+      <c r="C37" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="D37" s="1" t="str">
+        <v>Spectral Wolf</v>
+      </c>
+      <c r="E37" s="1" t="str">
+        <v>Spectral Wolf</v>
+      </c>
+      <c r="F37" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="n">
+        <v>6050</v>
+      </c>
+      <c r="B38" s="1" t="str">
+        <v>ObjectData MonsterCompanyName</v>
+      </c>
+      <c r="C38" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="D38" s="1" t="str">
+        <v>Spectral Wolves</v>
+      </c>
+      <c r="E38" s="1" t="str">
+        <v>Spectral Wolves</v>
+      </c>
+      <c r="F38" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="n">
+        <v>6051</v>
+      </c>
+      <c r="B39" s="1" t="str">
+        <v>UnitData Description</v>
+      </c>
+      <c r="C39" s="1" t="n">
+        <v>253</v>
+      </c>
+      <c r="D39" s="1" t="str">
+        <v>These spectral beasts are nightmares made manifest, given shape and form by the same shadowy magic used to call them forth. They are incorporeal and resistant to the harm caused by ordinary weapons, but are more easily disrupted by other forms of magic.</v>
+      </c>
+      <c r="E39" s="1" t="str">
+        <v>These spectral beasts are nightmares made manifest, given shape and form by the same shadowy magic used to call them forth. They are incorporeal and resistant to the harm caused by ordinary weapons, but are more easily disrupted by other forms of magic.</v>
+      </c>
+      <c r="F39" s="1" t="str">
+        <v>Zerin Summons Description</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="n">
+        <v>6052</v>
+      </c>
+      <c r="B40" s="1" t="str">
+        <v>UnitData Description</v>
+      </c>
+      <c r="C40" s="1" t="n">
+        <v>313</v>
+      </c>
+      <c r="D40" s="1" t="str">
+        <v>The Bone Reaver is the result of countless studies and experiments to perfect the creation of undead warriors. The components used to animate them, as well as the necessity of using quality corpses, has resulted in a far deadlier variant that is faster, sturdier and more expensive than their lesser counterparts.</v>
+      </c>
+      <c r="E40" s="1" t="str">
+        <v>The Bone Reaver is the result of countless studies and experiments to perfect the creation of undead warriors. The components used to animate them, as well as the necessity of using quality corpses, has resulted in a far deadlier variant that is faster, sturdier and more expensive than their lesser counterparts.</v>
+      </c>
+      <c r="F40" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="str">
+        <v># Buildings ==============================</v>
+      </c>
+      <c r="B41" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C41" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="n">
+        <v>6053</v>
+      </c>
+      <c r="B42" s="1" t="str">
+        <v>ObjectData ProperName</v>
+      </c>
+      <c r="C42" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D42" s="1" t="str">
+        <v>Cave</v>
+      </c>
+      <c r="E42" s="1" t="str">
+        <v>Cave</v>
+      </c>
+      <c r="F42" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="n">
+        <v>6054</v>
+      </c>
+      <c r="B43" s="1" t="str">
+        <v>ObjectData Description</v>
+      </c>
+      <c r="C43" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="D43" s="1" t="str">
+        <v>There is something unnatural about this cave.</v>
+      </c>
+      <c r="E43" s="1" t="str">
+        <v>There is something unnatural about this cave.</v>
+      </c>
+      <c r="F43" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="n">
+        <v>6055</v>
+      </c>
+      <c r="B44" s="1" t="str">
+        <v>ObjectData ProperName</v>
+      </c>
+      <c r="C44" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="D44" s="1" t="str">
+        <v>Ancient Abyss</v>
+      </c>
+      <c r="E44" s="1" t="str">
+        <v>Ancient Abyss</v>
+      </c>
+      <c r="F44" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="n">
+        <v>6056</v>
+      </c>
+      <c r="B45" s="1" t="str">
+        <v>ObjectData Description</v>
+      </c>
+      <c r="C45" s="1" t="n">
+        <v>159</v>
+      </c>
+      <c r="D45" s="1" t="str">
+        <v>A remnant of a Cataclysm in an age long past, infested with evil protecting their forgotten treasures. Only the prepared or foolish would dare venture near it.</v>
+      </c>
+      <c r="E45" s="1" t="str">
+        <v>A remnant of a Cataclysm in an age long past, infested with evil protecting their forgotten treasures. Only the prepared or foolish would dare venture near it.</v>
+      </c>
+      <c r="F45" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="n">
+        <v>6057</v>
+      </c>
+      <c r="B46" s="1" t="str">
+        <v>ObjectData ProperName</v>
+      </c>
+      <c r="C46" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="D46" s="1" t="str">
+        <v>Slaan Colony</v>
+      </c>
+      <c r="E46" s="1" t="str">
+        <v>Slaan Colony</v>
+      </c>
+      <c r="F46" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="n">
+        <v>6058</v>
+      </c>
+      <c r="B47" s="1" t="str">
+        <v>ObjectData ProperName</v>
+      </c>
+      <c r="C47" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="D47" s="1" t="str">
+        <v>Giant Wasp Hive</v>
+      </c>
+      <c r="E47" s="1" t="str">
+        <v>Giant Wasp Hive</v>
+      </c>
+      <c r="F47" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="str">
+        <v># Spells ==============================</v>
+      </c>
+      <c r="B48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F48" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="n">
+        <v>6059</v>
+      </c>
+      <c r="B49" s="1" t="str">
+        <v>ProperName</v>
+      </c>
+      <c r="C49" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="D49" s="1" t="str">
+        <v>Psalm of Fury</v>
+      </c>
+      <c r="E49" s="1" t="str">
+        <v>Psalm of Fury</v>
+      </c>
+      <c r="F49" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="n">
+        <v>6060</v>
+      </c>
+      <c r="B50" s="1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C50" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="D50" s="1" t="str">
+        <v>An exhortation that emboldens the caster's allies with speed and tenacity in battle.</v>
+      </c>
+      <c r="E50" s="1" t="str">
+        <v>An exhortation that emboldens the caster's allies with speed and tenacity in battle.</v>
+      </c>
+      <c r="F50" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="n">
+        <v>6061</v>
+      </c>
+      <c r="B51" s="1" t="str">
+        <v>ProperName</v>
+      </c>
+      <c r="C51" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="D51" s="1" t="str">
+        <v>Cold Snap</v>
+      </c>
+      <c r="E51" s="1" t="str">
+        <v>Cold Snap</v>
+      </c>
+      <c r="F51" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="n">
+        <v>6062</v>
+      </c>
+      <c r="B52" s="1" t="str">
+        <v>ProperName</v>
+      </c>
+      <c r="C52" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D52" s="1" t="str">
+        <v>Grit</v>
+      </c>
+      <c r="E52" s="1" t="str">
+        <v>Grit</v>
+      </c>
+      <c r="F52" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="n">
+        <v>6063</v>
+      </c>
+      <c r="B53" s="1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C53" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="D53" s="1" t="str">
+        <v>Through sheer force of will the caster is able to shrug off debilitating effects and effortlessly maneuver in difficult terrain.</v>
+      </c>
+      <c r="E53" s="1" t="str">
+        <v>Through sheer force of will the caster is able to shrug off debilitating effects and effortlessly maneuver in difficult terrain.</v>
+      </c>
+      <c r="F53" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="n">
+        <v>6064</v>
+      </c>
+      <c r="B54" s="1" t="str">
+        <v>ProperName</v>
+      </c>
+      <c r="C54" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="D54" s="1" t="str">
+        <v>True Grit</v>
+      </c>
+      <c r="E54" s="1" t="str">
+        <v>True Grit</v>
+      </c>
+      <c r="F54" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="n">
+        <v>6065</v>
+      </c>
+      <c r="B55" s="1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C55" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="D55" s="1" t="str">
+        <v>Through sheer force of will the caster is able to shrug off wounds and debilitating effects. Maneuvering in difficult terrain becomes effortless.</v>
+      </c>
+      <c r="E55" s="1" t="str">
+        <v>Through sheer force of will the caster is able to shrug off wounds and debilitating effects. Maneuvering in difficult terrain becomes effortless.</v>
+      </c>
+      <c r="F55" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="n">
+        <v>6066</v>
+      </c>
+      <c r="B56" s="1" t="str">
+        <v>ProperName</v>
+      </c>
+      <c r="C56" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="D56" s="1" t="str">
+        <v>Lightning Vestments</v>
+      </c>
+      <c r="E56" s="1" t="str">
+        <v>Lightning Vestments</v>
+      </c>
+      <c r="F56" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="n">
+        <v>6067</v>
+      </c>
+      <c r="B57" s="1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C57" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="D57" s="1" t="str">
+        <v>Wreaths the caster's comrades in crackling electricity that protects from physical attacks and harms those who dare to engage them in melee.</v>
+      </c>
+      <c r="E57" s="1" t="str">
+        <v>Wreaths the caster's comrades in crackling electricity that protects from physical attacks and harms those who dare to engage them in melee.</v>
+      </c>
+      <c r="F57" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="n">
+        <v>6068</v>
+      </c>
+      <c r="B58" s="1" t="str">
+        <v>ProperName</v>
+      </c>
+      <c r="C58" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="D58" s="1" t="str">
+        <v>Frenzy</v>
+      </c>
+      <c r="E58" s="1" t="str">
+        <v>Frenzy</v>
+      </c>
+      <c r="F58" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="n">
+        <v>6069</v>
+      </c>
+      <c r="B59" s="1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C59" s="1" t="n">
+        <v>143</v>
+      </c>
+      <c r="D59" s="1" t="str">
+        <v>The scent of blood drives the caster into a killing frenzy, leaving them open to attack as they hunt down their foes in a haze of red-hot rage.</v>
+      </c>
+      <c r="E59" s="1" t="str">
+        <v>The scent of blood drives the caster into a killing frenzy, leaving them open to attack as they hunt down their foes in a haze of red-hot rage.</v>
+      </c>
+      <c r="F59" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="n">
+        <v>6070</v>
+      </c>
+      <c r="B60" s="1" t="str">
+        <v>ProperName</v>
+      </c>
+      <c r="C60" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="D60" s="1" t="str">
+        <v>Spectral Veil</v>
+      </c>
+      <c r="E60" s="1" t="str">
+        <v>Spectral Veil</v>
+      </c>
+      <c r="F60" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="n">
+        <v>6071</v>
+      </c>
+      <c r="B61" s="1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C61" s="1" t="n">
+        <v>144</v>
+      </c>
+      <c r="D61" s="1" t="str">
+        <v>The black magicks of this spell temporarily turn the caster's comrades into ghostly shades, immaterial, and resistant to the weapons of mortals.</v>
+      </c>
+      <c r="E61" s="1" t="str">
+        <v>The black magicks of this spell temporarily turn the caster's comrades into ghostly shades, immaterial, and resistant to the weapons of mortals.</v>
+      </c>
+      <c r="F61" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="n">
+        <v>6072</v>
+      </c>
+      <c r="B62" s="1" t="str">
+        <v>ProperName</v>
+      </c>
+      <c r="C62" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="D62" s="1" t="str">
+        <v>Shadowstun</v>
+      </c>
+      <c r="E62" s="1" t="str">
+        <v>Shadowstun</v>
+      </c>
+      <c r="F62" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="n">
+        <v>6073</v>
+      </c>
+      <c r="B63" s="1" t="str">
+        <v>ProperName</v>
+      </c>
+      <c r="C63" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="D63" s="1" t="str">
+        <v>Grasping Vines</v>
+      </c>
+      <c r="E63" s="1" t="str">
+        <v>Grasping Vines</v>
+      </c>
+      <c r="F63" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="n">
+        <v>6074</v>
+      </c>
+      <c r="B64" s="1" t="str">
+        <v>ProperName</v>
+      </c>
+      <c r="C64" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="D64" s="1" t="str">
+        <v>Overgrowth</v>
+      </c>
+      <c r="E64" s="1" t="str">
+        <v>Overgrowth</v>
+      </c>
+      <c r="F64" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="n">
+        <v>6075</v>
+      </c>
+      <c r="B65" s="1" t="str">
+        <v>ProperName</v>
+      </c>
+      <c r="C65" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="D65" s="1" t="str">
+        <v>Cantrip</v>
+      </c>
+      <c r="E65" s="1" t="str">
+        <v>Cantrip</v>
+      </c>
+      <c r="F65" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="n">
+        <v>6076</v>
+      </c>
+      <c r="B66" s="1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C66" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="D66" s="1" t="str">
+        <v>A controlled burst of energy erupts from the mage's fingertips and flies towards an enemy.</v>
+      </c>
+      <c r="E66" s="1" t="str">
+        <v>A controlled burst of energy erupts from the mage's fingertips and flies towards an enemy.</v>
+      </c>
+      <c r="F66" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="n">
+        <v>6077</v>
+      </c>
+      <c r="B67" s="1" t="str">
+        <v>ProperName</v>
+      </c>
+      <c r="C67" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="D67" s="1" t="str">
+        <v>Summon Magma Elemental</v>
+      </c>
+      <c r="E67" s="1" t="str">
+        <v>Summon Magma Elemental</v>
+      </c>
+      <c r="F67" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="n">
+        <v>6078</v>
+      </c>
+      <c r="B68" s="1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C68" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="D68" s="1" t="str">
+        <v>Summons forth an elemental beast of flame to do the caster's bidding.</v>
+      </c>
+      <c r="E68" s="1" t="str">
+        <v>Summons forth an elemental beast of flame to do the caster's bidding.</v>
+      </c>
+      <c r="F68" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="n">
+        <v>6079</v>
+      </c>
+      <c r="B69" s="1" t="str">
+        <v>ProperName</v>
+      </c>
+      <c r="C69" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="D69" s="1" t="str">
+        <v>Magmatic Summons</v>
+      </c>
+      <c r="E69" s="1" t="str">
+        <v>Magmatic Summons</v>
+      </c>
+      <c r="F69" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="n">
+        <v>6080</v>
+      </c>
+      <c r="B70" s="1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="D70" s="1" t="str">
+        <v>Summons forth a pair of magma elementals to do the caster's bidding.</v>
+      </c>
+      <c r="E70" s="1" t="str">
+        <v>Summons forth a pair of magma elementals to do the caster's bidding.</v>
+      </c>
+      <c r="F70" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="n">
+        <v>6081</v>
+      </c>
+      <c r="B71" s="1" t="str">
+        <v>ProperName</v>
+      </c>
+      <c r="C71" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="D71" s="1" t="str">
+        <v>Lava Burst</v>
+      </c>
+      <c r="E71" s="1" t="str">
+        <v>Lava Burst</v>
+      </c>
+      <c r="F71" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="n">
+        <v>6082</v>
+      </c>
+      <c r="B72" s="1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C72" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="D72" s="1" t="str">
+        <v>A searing burst of lava and choking ash.</v>
+      </c>
+      <c r="E72" s="1" t="str">
+        <v>A searing burst of lava and choking ash.</v>
+      </c>
+      <c r="F72" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="n">
+        <v>6083</v>
+      </c>
+      <c r="B73" s="1" t="str">
+        <v>ProperName</v>
+      </c>
+      <c r="C73" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="D73" s="1" t="str">
+        <v>Summon Spectral Wolves</v>
+      </c>
+      <c r="E73" s="1" t="str">
+        <v>Summon Spectral Wolves</v>
+      </c>
+      <c r="F73" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="n">
+        <v>6084</v>
+      </c>
+      <c r="B74" s="1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C74" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="D74" s="1" t="str">
+        <v>Summons forth a pair of ghostly wolves to enforce the caster's will.</v>
+      </c>
+      <c r="E74" s="1" t="str">
+        <v>Summons forth a pair of ghostly wolves to enforce the caster's will.</v>
+      </c>
+      <c r="F74" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="n">
+        <v>6085</v>
+      </c>
+      <c r="B75" s="1" t="str">
+        <v>ProperName</v>
+      </c>
+      <c r="C75" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="D75" s="1" t="str">
+        <v>Ethereal Form</v>
+      </c>
+      <c r="E75" s="1" t="str">
+        <v>Ethereal Form</v>
+      </c>
+      <c r="F75" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="n">
+        <v>6086</v>
+      </c>
+      <c r="B76" s="1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C76" s="1" t="n">
+        <v>106</v>
+      </c>
+      <c r="D76" s="1" t="str">
+        <v>The spectral wolf stays partly intangible, causing ordinary weapons to pass through it with little effect.</v>
+      </c>
+      <c r="E76" s="1" t="str">
+        <v>The spectral wolf stays partly intangible, causing ordinary weapons to pass through it with little effect.</v>
+      </c>
+      <c r="F76" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="n">
+        <v>6087</v>
+      </c>
+      <c r="B77" s="1" t="str">
+        <v>ProperName</v>
+      </c>
+      <c r="C77" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="D77" s="1" t="str">
+        <v>Soul Rend</v>
+      </c>
+      <c r="E77" s="1" t="str">
+        <v>Soul Rend</v>
+      </c>
+      <c r="F77" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="n">
+        <v>6088</v>
+      </c>
+      <c r="B78" s="1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C78" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="D78" s="1" t="str">
+        <v>Spectral claws rend flesh and scar the spirit, leaving their prey fearful and weak.</v>
+      </c>
+      <c r="E78" s="1" t="str">
+        <v>Spectral claws rend flesh and scar the spirit, leaving their prey fearful and weak.</v>
+      </c>
+      <c r="F78" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="n">
+        <v>6089</v>
+      </c>
+      <c r="B79" s="1" t="str">
+        <v>ProperName</v>
+      </c>
+      <c r="C79" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="D79" s="1" t="str">
+        <v>Summon Phage Spider</v>
+      </c>
+      <c r="E79" s="1" t="str">
+        <v>Summon Phage Spider</v>
+      </c>
+      <c r="F79" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="n">
+        <v>6090</v>
+      </c>
+      <c r="B80" s="1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C80" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="D80" s="1" t="str">
+        <v>Summons forth a hideous Phage Spider to enforce the caster's will.</v>
+      </c>
+      <c r="E80" s="1" t="str">
+        <v>Summons forth a hideous Phage Spider to enforce the caster's will.</v>
+      </c>
+      <c r="F80" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="n">
+        <v>6091</v>
+      </c>
+      <c r="B81" s="1" t="str">
+        <v>ProperName</v>
+      </c>
+      <c r="C81" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="D81" s="1" t="str">
+        <v>Arachnid Swarm</v>
+      </c>
+      <c r="E81" s="1" t="str">
+        <v>Arachnid Swarm</v>
+      </c>
+      <c r="F81" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="n">
+        <v>6092</v>
+      </c>
+      <c r="B82" s="1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C82" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="D82" s="1" t="str">
+        <v>Summons forth a pair of hideous Phage Spiders to enforce the caster's will.</v>
+      </c>
+      <c r="E82" s="1" t="str">
+        <v>Summons forth a pair of hideous Phage Spiders to enforce the caster's will.</v>
+      </c>
+      <c r="F82" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="n">
+        <v>6093</v>
+      </c>
+      <c r="B83" s="1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C83" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="D83" s="1" t="str">
+        <v>The phage spider stays partly intangible, causing ordinary weapons to pass through it with little effect.</v>
+      </c>
+      <c r="E83" s="1" t="str">
+        <v>The phage spider stays partly intangible, causing ordinary weapons to pass through it with little effect.</v>
+      </c>
+      <c r="F83" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="n">
+        <v>6094</v>
+      </c>
+      <c r="B84" s="1" t="str">
+        <v>ProperName</v>
+      </c>
+      <c r="C84" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="D84" s="1" t="str">
+        <v>Gloom Webbing</v>
+      </c>
+      <c r="E84" s="1" t="str">
+        <v>Gloom Webbing</v>
+      </c>
+      <c r="F84" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="n">
+        <v>6095</v>
+      </c>
+      <c r="B85" s="1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C85" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="D85" s="1" t="str">
+        <v>Shoots a splatter of silk at a target, immobilizing it and sapping morale.</v>
+      </c>
+      <c r="E85" s="1" t="str">
+        <v>Shoots a splatter of silk at a target, immobilizing it and sapping morale.</v>
+      </c>
+      <c r="F85" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="n">
+        <v>6096</v>
+      </c>
+      <c r="B86" s="1" t="str">
+        <v>ProperName</v>
+      </c>
+      <c r="C86" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="D86" s="1" t="str">
+        <v>Ill Omen</v>
+      </c>
+      <c r="E86" s="1" t="str">
+        <v>Ill Omen</v>
+      </c>
+      <c r="F86" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="n">
+        <v>6097</v>
+      </c>
+      <c r="B87" s="1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C87" s="1" t="n">
+        <v>122</v>
+      </c>
+      <c r="D87" s="1" t="str">
+        <v>The caster brands their enemies with dark sigils that sap strength and resolve, leaving weeping wounds that will not heal.</v>
+      </c>
+      <c r="E87" s="1" t="str">
+        <v>The caster brands their enemies with dark sigils that sap strength and resolve, leaving weeping wounds that will not heal.</v>
+      </c>
+      <c r="F87" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="n">
+        <v>6098</v>
+      </c>
+      <c r="B88" s="1" t="str">
+        <v>ProperName</v>
+      </c>
+      <c r="C88" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="D88" s="1" t="str">
+        <v>Fallen Star</v>
+      </c>
+      <c r="E88" s="1" t="str">
+        <v>Fallen Star</v>
+      </c>
+      <c r="F88" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="n">
+        <v>6099</v>
+      </c>
+      <c r="B89" s="1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C89" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="D89" s="1" t="str">
+        <v>With a supreme display of arcane skill, the caster is able to bring forth a titanic meteor from the skies to obliterate their enemies.</v>
+      </c>
+      <c r="E89" s="1" t="str">
+        <v>With a supreme display of arcane skill, the caster is able to bring forth a titanic meteor from the skies to obliterate their enemies.</v>
+      </c>
+      <c r="F89" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="n">
+        <v>6100</v>
+      </c>
+      <c r="B90" s="1" t="str">
+        <v>ProperName</v>
+      </c>
+      <c r="C90" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="D90" s="1" t="str">
+        <v>Spirited Charge</v>
+      </c>
+      <c r="E90" s="1" t="str">
+        <v>Spirited Charge</v>
+      </c>
+      <c r="F90" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="n">
+        <v>6101</v>
+      </c>
+      <c r="B91" s="1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C91" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="D91" s="1" t="str">
+        <v>With precision and incredible power, the rider skewers their foe with a glorious charge.</v>
+      </c>
+      <c r="E91" s="1" t="str">
+        <v>With precision and incredible power, the rider skewers their foe with a glorious charge.</v>
+      </c>
+      <c r="F91" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="n">
+        <v>6102</v>
+      </c>
+      <c r="B92" s="1" t="str">
+        <v>ProperName</v>
+      </c>
+      <c r="C92" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="D92" s="1" t="str">
+        <v>Scorching Blast</v>
+      </c>
+      <c r="E92" s="1" t="str">
+        <v>Scorching Blast</v>
+      </c>
+      <c r="F92" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="n">
+        <v>6103</v>
+      </c>
+      <c r="B93" s="1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C93" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="D93" s="1" t="str">
+        <v>Generates a white-hot ball of searing flames that shoots out and strikes an opponent.</v>
+      </c>
+      <c r="E93" s="1" t="str">
+        <v>Generates a white-hot ball of searing flames that shoots out and strikes an opponent.</v>
+      </c>
+      <c r="F93" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="n">
+        <v>6104</v>
+      </c>
+      <c r="B94" s="1" t="str">
+        <v>ProperName</v>
+      </c>
+      <c r="C94" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="D94" s="1" t="str">
+        <v>Gray Waste</v>
+      </c>
+      <c r="E94" s="1" t="str">
+        <v>Gray Waste</v>
+      </c>
+      <c r="F94" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="n">
+        <v>6105</v>
+      </c>
+      <c r="B95" s="1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C95" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="D95" s="1" t="str">
+        <v>Creates a crippling cloud of darkness that leaves enemies caught within enfeebled in both body and mind.</v>
+      </c>
+      <c r="E95" s="1" t="str">
+        <v>Creates a crippling cloud of darkness that leaves enemies caught within enfeebled in both body and mind.</v>
+      </c>
+      <c r="F95" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="n">
+        <v>6106</v>
+      </c>
+      <c r="B96" s="1" t="str">
+        <v>ProperName</v>
+      </c>
+      <c r="C96" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="D96" s="1" t="str">
+        <v>Litany of Banishment</v>
+      </c>
+      <c r="E96" s="1" t="str">
+        <v>Litany of Banishment</v>
+      </c>
+      <c r="F96" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="1" t="n">
+        <v>6107</v>
+      </c>
+      <c r="B97" s="1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C97" s="1" t="n">
+        <v>138</v>
+      </c>
+      <c r="D97" s="1" t="str">
+        <v>This sacred chant emits a burst of radiance that strikes out against creatures of shadow, leaving them vulnerable to further holy attacks.</v>
+      </c>
+      <c r="E97" s="1" t="str">
+        <v>This sacred chant emits a burst of radiance that strikes out against creatures of shadow, leaving them vulnerable to further holy attacks.</v>
+      </c>
+      <c r="F97" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="1" t="n">
+        <v>6108</v>
+      </c>
+      <c r="B98" s="1" t="str">
+        <v>ProperName</v>
+      </c>
+      <c r="C98" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="D98" s="1" t="str">
+        <v>Rallying Call</v>
+      </c>
+      <c r="E98" s="1" t="str">
+        <v>Rallying Call</v>
+      </c>
+      <c r="F98" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="1" t="n">
+        <v>6109</v>
+      </c>
+      <c r="B99" s="1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C99" s="1" t="n">
+        <v>102</v>
+      </c>
+      <c r="D99" s="1" t="str">
+        <v>Leads the company in a glorious charge, inspiring them to greater feats of tenacity and determination.</v>
+      </c>
+      <c r="E99" s="1" t="str">
+        <v>Leads the company in a glorious charge, inspiring them to greater feats of tenacity and determination.</v>
+      </c>
+      <c r="F99" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="1" t="str">
+        <v># BONUS.INI ==============================</v>
+      </c>
+      <c r="B100" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C100" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D100" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E100" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F100" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="1" t="n">
+        <v>6110</v>
+      </c>
+      <c r="B101" s="1" t="str">
+        <v>ATTACK_BONUS_TO_SHADOW name2</v>
+      </c>
+      <c r="C101" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="D101" s="1" t="str">
+        <v>Nyctophobia</v>
+      </c>
+      <c r="E101" s="1" t="str">
+        <v>Nyctophobia</v>
+      </c>
+      <c r="F101" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="1" t="n">
+        <v>6111</v>
+      </c>
+      <c r="B102" s="1" t="str">
+        <v>ATTACK_BONUS_TO_SHADOW Description2</v>
+      </c>
+      <c r="C102" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="D102" s="1" t="str">
+        <v>Decreases attacks against shadow elements by %+d.</v>
+      </c>
+      <c r="E102" s="1" t="str">
+        <v>Decreases attacks against shadow elements by %+d.</v>
+      </c>
+      <c r="F102" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="1" t="n">
+        <v>6112</v>
+      </c>
+      <c r="B103" s="1" t="str">
+        <v>ATTACK_BONUS_TO_NONSHADOW Description1</v>
+      </c>
+      <c r="C103" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="D103" s="1" t="str">
+        <v>Increases attacks against non-shadow elements by %+d.</v>
+      </c>
+      <c r="E103" s="1" t="str">
+        <v>Increases attacks against non-shadow elements by %+d.</v>
+      </c>
+      <c r="F103" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="1" t="str">
+        <v># COMPONENTS.INI ==============================</v>
+      </c>
+      <c r="B104" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C104" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D104" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E104" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F104" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="1" t="n">
+        <v>6113</v>
+      </c>
+      <c r="B105" s="1" t="str">
+        <v>MiningPost Description</v>
+      </c>
+      <c r="C105" s="1" t="n">
+        <v>119</v>
+      </c>
+      <c r="D105" s="1" t="str">
+        <v>The mining post trains local workers to gather and process stone resources. Provides an additional +4 Stone per minute.</v>
+      </c>
+      <c r="E105" s="1" t="str">
+        <v>The mining post trains local workers to gather and process stone resources. Provides an additional +4 Stone per minute.</v>
+      </c>
+      <c r="F105" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="1" t="n">
+        <v>6114</v>
+      </c>
+      <c r="B106" s="1" t="str">
+        <v>MasonryGuild Description</v>
+      </c>
+      <c r="C106" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="D106" s="1" t="str">
+        <v>The masonry guild repairs damage done to the settlement automatically and reduces commission costs for Engineers by 40%.</v>
+      </c>
+      <c r="E106" s="1" t="str">
+        <v>The masonry guild repairs damage done to the settlement automatically and reduces commission costs for Engineers by 40%.</v>
+      </c>
+      <c r="F106" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="1" t="n">
+        <v>6115</v>
+      </c>
+      <c r="B107" s="1" t="str">
+        <v>StoneMarket Description</v>
+      </c>
+      <c r="C107" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="D107" s="1" t="str">
+        <v>The stone export sells off 5 Stone produced by the quarry for +5 Gold per minute.</v>
+      </c>
+      <c r="E107" s="1" t="str">
+        <v>The stone export sells off 5 Stone produced by the quarry for +5 Gold per minute.</v>
+      </c>
+      <c r="F107" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="1" t="n">
+        <v>6116</v>
+      </c>
+      <c r="B108" s="1" t="str">
+        <v>Sawmill Description</v>
+      </c>
+      <c r="C108" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="D108" s="1" t="str">
+        <v>Advanced saw blades process timber faster than a normal woodmill. Provides an additional +4 Wood per minute.</v>
+      </c>
+      <c r="E108" s="1" t="str">
+        <v>Advanced saw blades process timber faster than a normal woodmill. Provides an additional +4 Wood per minute.</v>
+      </c>
+      <c r="F108" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="1" t="n">
+        <v>6117</v>
+      </c>
+      <c r="B109" s="1" t="str">
+        <v>WoodMarket Description</v>
+      </c>
+      <c r="C109" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="D109" s="1" t="str">
+        <v>The wood export sells off 5 Wood produced by the woodmill for +10 Gold per minute.</v>
+      </c>
+      <c r="E109" s="1" t="str">
+        <v>The wood export sells off 5 Wood produced by the woodmill for +10 Gold per minute.</v>
+      </c>
+      <c r="F109" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="1" t="n">
+        <v>6118</v>
+      </c>
+      <c r="B110" s="1" t="str">
+        <v>BlastFurnace Description</v>
+      </c>
+      <c r="C110" s="1" t="n">
+        <v>111</v>
+      </c>
+      <c r="D110" s="1" t="str">
+        <v>An upgraded form of blacksmith with a larger, more advanced furnace. Provides an additional +4 Iron per minute.</v>
+      </c>
+      <c r="E110" s="1" t="str">
+        <v>An upgraded form of blacksmith with a larger, more advanced furnace. Provides an additional +4 Iron per minute.</v>
+      </c>
+      <c r="F110" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="1" t="n">
+        <v>6119</v>
+      </c>
+      <c r="B111" s="1" t="str">
+        <v>ArmoryGuild Description</v>
+      </c>
+      <c r="C111" s="1" t="n">
+        <v>121</v>
+      </c>
+      <c r="D111" s="1" t="str">
+        <v>Reduces commission cost for Infantry, Grenadiers, Dragoons, and Elite units by 50%. Increases militia attack value by +2.</v>
+      </c>
+      <c r="E111" s="1" t="str">
+        <v>Reduces commission cost for Infantry, Grenadiers, Dragoons, and Elite units by 50%. Increases militia attack value by +2.</v>
+      </c>
+      <c r="F111" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="1" t="n">
+        <v>6120</v>
+      </c>
+      <c r="B112" s="1" t="str">
+        <v>IronMarket Description</v>
+      </c>
+      <c r="C112" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="D112" s="1" t="str">
+        <v>The iron export sells off 5 Iron produced by the blacksmith for +15 Gold per minute.</v>
+      </c>
+      <c r="E112" s="1" t="str">
+        <v>The iron export sells off 5 Iron produced by the blacksmith for +15 Gold per minute.</v>
+      </c>
+      <c r="F112" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="1" t="n">
+        <v>6121</v>
+      </c>
+      <c r="B113" s="1" t="str">
+        <v>Billet Description</v>
+      </c>
+      <c r="C113" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="D113" s="1" t="str">
+        <v>A billet finds recruits and organizes them. This creates a 33% reduction in commission cost for all companies recruited here.</v>
+      </c>
+      <c r="E113" s="1" t="str">
+        <v>A billet finds recruits and organizes them. This creates a 33% reduction in commission cost for all companies recruited here.</v>
+      </c>
+      <c r="F113" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="1" t="n">
+        <v>6122</v>
+      </c>
+      <c r="B114" s="1" t="str">
+        <v>Temple Description</v>
+      </c>
+      <c r="C114" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="D114" s="1" t="str">
+        <v>Provides your kingdom with +2 Iron and +2 Mana per minute.</v>
+      </c>
+      <c r="E114" s="1" t="str">
+        <v>Provides your kingdom with +2 Iron and +2 Mana per minute.</v>
+      </c>
+      <c r="F114" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="1" t="n">
+        <v>6123</v>
+      </c>
+      <c r="B115" s="1" t="str">
+        <v>MageCollege Description</v>
+      </c>
+      <c r="C115" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="D115" s="1" t="str">
+        <v>The mage college is an institute of higher learning and much experimentation. Provides an additional +4 Mana per minute.</v>
+      </c>
+      <c r="E115" s="1" t="str">
+        <v>The mage college is an institute of higher learning and much experimentation. Provides an additional +4 Mana per minute.</v>
+      </c>
+      <c r="F115" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="1" t="n">
+        <v>6124</v>
+      </c>
+      <c r="B116" s="1" t="str">
+        <v>TurretedRamparts Description</v>
+      </c>
+      <c r="C116" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="D116" s="1" t="str">
+        <v>A blend of fortification and watch towers, turreted ramparts house additional militia and increase the visual range of the city.</v>
+      </c>
+      <c r="E116" s="1" t="str">
+        <v>A blend of fortification and watch towers, turreted ramparts house additional militia and increase the visual range of the city.</v>
+      </c>
+      <c r="F116" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="1" t="str">
+        <v># Adtl items</v>
+      </c>
+      <c r="B117" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C117" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D117" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E117" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F117" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="1" t="n">
+        <v>6125</v>
+      </c>
+      <c r="B118" s="1" t="str">
+        <v>UnitData Description</v>
+      </c>
+      <c r="C118" s="1" t="n">
+        <v>471</v>
+      </c>
+      <c r="D118" s="1" t="str">
+        <v>Amon Koth was not originally condemned as Ceyah Kohan during the initial purge. He willingly chose exile and followed after some of the other Ceyah Kohan that had been ostracized. He eventually found himself deep underground and separated from all of the other Ceyah Kohan. It was here that he somehow spawned his 'children', the Rhaksha. No one knows how he managed this, or why. He has established himself as their god and master, and continues to rule over them still.</v>
+      </c>
+      <c r="E118" s="1" t="str">
+        <v>Amon Koth was not originally condemned as Ceyah Kohan during the initial purge. He willingly chose exile and followed after some of the other Ceyah Kohan that had been ostracized. He eventually found himself deep underground and separated from all of the other Ceyah Kohan. It was here that he somehow spawned his 'children', the Rhaksha. No one knows how he managed this, or why. He has established himself as their god and master, and continues to rule over them still.</v>
+      </c>
+      <c r="F118" s="1" t="str">
+        <v>Amon Koth Description</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="1" t="n">
+        <v>6126</v>
+      </c>
+      <c r="B119" s="1" t="str">
+        <v>UnitData Description</v>
+      </c>
+      <c r="C119" s="1" t="n">
+        <v>763</v>
+      </c>
+      <c r="D119" s="1" t="str">
+        <v>One of the true Ceyah Kohan who broke from the High Council on the Day of Betrayal. Shohn Maht was a lesser council member who idolized Ceyahdev and strove to be as strong and influential as her. When Ceyahdev broke from the Council, Shohn Maht followed without hesitation. He embraced his banishment, convincing himself that he was superior to the rest of the Kohan. He followed Ceyahdev for a short time, then broke away when it became apparent that she only desired isolation. Shohn Maht desired power and decided that the Mareten would make perfect subjects. He managed to survive the next cataclysm and learned as much as he could about Ahriman and his plans. He is a master of dark magic and much of his kingdom is protected with hordes of the walking dead.</v>
+      </c>
+      <c r="E119" s="1" t="str">
+        <v>One of the true Ceyah Kohan who broke from the High Council on the Day of Betrayal. Shohn Maht was a lesser council member who idolized Ceyahdev and strove to be as strong and influential as her. When Ceyahdev broke from the Council, Shohn Maht followed without hesitation. He embraced his banishment, convincing himself that he was superior to the rest of the Kohan. He followed Ceyahdev for a short time, then broke away when it became apparent that she only desired isolation. Shohn Maht desired power and decided that the Mareten would make perfect subjects. He managed to survive the next cataclysm and learned as much as he could about Ahriman and his plans. He is a master of dark magic and much of his kingdom is protected with hordes of the walking dead.</v>
+      </c>
+      <c r="F119" s="1" t="str">
+        <v>Shohn Maht Description</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="1" t="n">
+        <v>6127</v>
+      </c>
+      <c r="B120" s="1" t="str">
+        <v>UnitData Description</v>
+      </c>
+      <c r="C120" s="1" t="n">
+        <v>459</v>
+      </c>
+      <c r="D120" s="1" t="str">
+        <v>Ashavir is a true mercenary. He changes sides the moment he sees greater opportunity in the other camp. Known for his handsome appearance and his seductive ways, Ashavir is perhaps the most selfish of all Ceyah, caring nothing for political or religious ideals. He has even been known to work for Nationalist concerns against the Ceyah Lords. Even so, Ahriman has blessed him with great power, though none of the other Ceyah can fathom the reason behind this.</v>
+      </c>
+      <c r="E120" s="1" t="str">
+        <v>Ashavir is a true mercenary. He changes sides the moment he sees greater opportunity in the other camp. Known for his handsome appearance and his seductive ways, Ashavir is perhaps the most selfish of all Ceyah, caring nothing for political or religious ideals. He has even been known to work for Nationalist concerns against the Ceyah Lords. Even so, Ahriman has blessed him with great power, though none of the other Ceyah can fathom the reason behind this.</v>
+      </c>
+      <c r="F120" s="1" t="str">
+        <v>Ashavir Description</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="1" t="n">
+        <v>6128</v>
+      </c>
+      <c r="B121" s="1" t="str">
+        <v>UnitData Description</v>
+      </c>
+      <c r="C121" s="1" t="n">
+        <v>340</v>
+      </c>
+      <c r="D121" s="1" t="str">
+        <v>Hasanko is a dangerous and power-hungry Ceyah who sees himself rising above the even the first Ceyah Lords. Despite being dedicated to Ahriman, he constantly plots against his brethren. He always appears in the field of combat as a monstrous spectral knight, although it is unknown how he does this, whether through illusion or other means.</v>
+      </c>
+      <c r="E121" s="1" t="str">
+        <v>Hasanko is a dangerous and power-hungry Ceyah who sees himself rising above the even the first Ceyah Lords. Despite being dedicated to Ahriman, he constantly plots against his brethren. He always appears in the field of combat as a monstrous spectral knight, although it is unknown how he does this, whether through illusion or other means.</v>
+      </c>
+      <c r="F121" s="1" t="str">
+        <v>Hasanko Description</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="1" t="n">
+        <v>6129</v>
+      </c>
+      <c r="B122" s="1" t="str">
+        <v>UnitData Description</v>
+      </c>
+      <c r="C122" s="1" t="n">
+        <v>348</v>
+      </c>
+      <c r="D122" s="1" t="str">
+        <v>The Mercenary is a fast and deadly rogue infantryman who works for the highest bidder. They will maintain their own equipment and upkeep but are expensive and not known for having high morale. Their status as contractors, as well as their separate logistics, prevents them from making use of many - if any at all - of their employer's technologies.</v>
+      </c>
+      <c r="E122" s="1" t="str">
+        <v>The Mercenary is a fast and deadly rogue infantryman who works for the highest bidder. They will maintain their own equipment and upkeep but are expensive and not known for having high morale. Their status as contractors, as well as their separate logistics, prevents them from making use of many - if any at all - of their employer's technologies.</v>
+      </c>
+      <c r="F122" s="1" t="str">
+        <v>Mercenary Description</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="1" t="n">
+        <v>6130</v>
+      </c>
+      <c r="B123" s="1" t="str">
+        <v>UnitData Description</v>
+      </c>
+      <c r="C123" s="1" t="n">
+        <v>163</v>
+      </c>
+      <c r="D123" s="1" t="str">
+        <v>Gifted by the Nightbringer with the ability to force enemies into nightmare-filled sleep, the Shadow Prophet is one of the most feared of the Nightbringer priests.</v>
+      </c>
+      <c r="E123" s="1" t="str">
+        <v>Gifted by the Nightbringer with the ability to force enemies into nightmare-filled sleep, the Shadow Prophet is one of the most feared of the Nightbringer priests.</v>
+      </c>
+      <c r="F123" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="1" t="n">
+        <v>6131</v>
+      </c>
+      <c r="B124" s="1" t="str">
+        <v>HIT_POINTS_BONUS name2</v>
+      </c>
+      <c r="C124" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="D124" s="1" t="str">
+        <v>Sickly</v>
+      </c>
+      <c r="E124" s="1" t="str">
+        <v>Sickly</v>
+      </c>
+      <c r="F124" s="1" t="str">
+        <v>Bonus Name</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="1" t="n">
+        <v>6132</v>
+      </c>
+      <c r="B125" s="1" t="str">
+        <v>UPGRADE_BONUS_COST_GROUP_3 name2</v>
+      </c>
+      <c r="C125" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="D125" s="1" t="str">
+        <v>Engineer Elements</v>
+      </c>
+      <c r="E125" s="1" t="str">
+        <v>Engineer Elements</v>
+      </c>
+      <c r="F125" s="1" t="str">
+        <v>Bonus Name</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="1" t="n">
+        <v>6133</v>
+      </c>
+      <c r="B126" s="1" t="str">
+        <v>UPGRADE_BONUS_COST_GROUP_3 Description2</v>
+      </c>
+      <c r="C126" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="D126" s="1" t="str">
+        <v>Engineer Commission costs are reduced to %d%% of normal.</v>
+      </c>
+      <c r="E126" s="1" t="str">
+        <v>Engineer Commission costs are reduced to %d%% of normal.</v>
+      </c>
+      <c r="F126" s="1" t="str">
+        <v>Bonus Description</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="1" t="n">
+        <v>6134</v>
+      </c>
+      <c r="B127" s="1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C127" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="D127" s="1" t="str">
+        <v>A concussive blast of arctic air that freezes a target in their tracks. The frozen target is more susceptible to damage.</v>
+      </c>
+      <c r="E127" s="1" t="str">
+        <v>A concussive blast of arctic air that freezes a target in their tracks. The frozen target is more susceptible to damage.</v>
+      </c>
+      <c r="F127" s="1" t="str">
+        <v>Ice Storm Spell Description</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="1" t="n">
+        <v>6135</v>
+      </c>
+      <c r="B128" s="1" t="str">
+        <v>ATTACK_BONUS_TO_NONSHADOW Description2</v>
+      </c>
+      <c r="C128" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="D128" s="1" t="str">
+        <v>Decreases attacks against non-shadow elements by %+d.</v>
+      </c>
+      <c r="E128" s="1" t="str">
+        <v>Decreases attacks against non-shadow elements by %+d.</v>
+      </c>
+      <c r="F128" s="1" t="str">
+        <v>Bonus Description</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="1" t="n">
+        <v>6136</v>
+      </c>
+      <c r="B129" s="1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C129" s="1" t="n">
+        <v>158</v>
+      </c>
+      <c r="D129" s="1" t="str">
+        <v>Purple mists engulf the mage's targets, causing them to move as though walking through thick mud. Affected targets move, attack and defend slower than normal.</v>
+      </c>
+      <c r="E129" s="1" t="str">
+        <v>Purple mists engulf the mage's targets, causing them to move as though walking through thick mud. Affected targets move, attack and defend slower than normal.</v>
+      </c>
+      <c r="F129" s="1" t="str">
+        <v>Slow Spell Description</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="1" t="str">
+        <v>#Technology.ini===================================</v>
+      </c>
+      <c r="B130" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C130" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D130" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E130" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F130" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="1" t="n">
+        <v>6137</v>
+      </c>
+      <c r="B131" s="1" t="str">
+        <v>Pathfinder Description</v>
+      </c>
+      <c r="C131" s="1" t="n">
+        <v>164</v>
+      </c>
+      <c r="D131" s="1" t="str">
+        <v>Pathfinders are specially trained, elite members of the secret Ranger society. Requires a Woodmill and Library to recruit. Cannot be recruited in Ceyah settlements.</v>
+      </c>
+      <c r="E131" s="1" t="str">
+        <v>Pathfinders are specially trained, elite members of the secret Ranger society. Requires a Woodmill and Library to recruit. Cannot be recruited in Ceyah settlements.</v>
+      </c>
+      <c r="F131" s="1" t="str">
+        <v>Technology Description</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="1" t="n">
+        <v>6138</v>
+      </c>
+      <c r="B132" s="1" t="str">
+        <v>Lich Description</v>
+      </c>
+      <c r="C132" s="1" t="n">
+        <v>155</v>
+      </c>
+      <c r="D132" s="1" t="str">
+        <v>The lich is a special form of Wraith, even more terrifying in power and capacity for evil. Requires a Ceyah Settlement, Mana Forge, and Library to recruit.</v>
+      </c>
+      <c r="E132" s="1" t="str">
+        <v>The lich is a special form of Wraith, even more terrifying in power and capacity for evil. Requires a Ceyah Settlement, Mana Forge, and Library to recruit.</v>
+      </c>
+      <c r="F132" s="1" t="str">
+        <v>Technology Description</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="1" t="n">
+        <v>6139</v>
+      </c>
+      <c r="B133" s="1" t="str">
+        <v>Enchanter Description</v>
+      </c>
+      <c r="C133" s="1" t="n">
+        <v>182</v>
+      </c>
+      <c r="D133" s="1" t="str">
+        <v>Enchanters are the masters of spell manipulation. They can both protect their own troops from spells and make spells more effective on enemies. Requires an Astrology Hall to recruit.</v>
+      </c>
+      <c r="E133" s="1" t="str">
+        <v>Enchanters are the masters of spell manipulation. They can both protect their own troops from spells and make spells more effective on enemies. Requires an Astrology Hall to recruit.</v>
+      </c>
+      <c r="F133" s="1" t="str">
+        <v>Technology Description</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="1" t="n">
+        <v>6140</v>
+      </c>
+      <c r="B134" s="1" t="str">
+        <v>Conjuror Description</v>
+      </c>
+      <c r="C134" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="D134" s="1" t="str">
+        <v>Conjurors have delved into the dark side of summoning, able to summon creatures of shadow to fight for them. Requires an Astrology Hall to recruit.</v>
+      </c>
+      <c r="E134" s="1" t="str">
+        <v>Conjurors have delved into the dark side of summoning, able to summon creatures of shadow to fight for them. Requires an Astrology Hall to recruit.</v>
+      </c>
+      <c r="F134" s="1" t="str">
+        <v>Technology Description</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="1" t="n">
+        <v>6141</v>
+      </c>
+      <c r="B135" s="1" t="str">
+        <v>Devout Description</v>
+      </c>
+      <c r="C135" s="1" t="n">
+        <v>209</v>
+      </c>
+      <c r="D135" s="1" t="str">
+        <v>These priestesses have been so warped by their channeling of dark powers that they have become insane fanatics, capable of wielding terrifying spells. Requires a Ceyah settlement and a Nightbringer to recruit.</v>
+      </c>
+      <c r="E135" s="1" t="str">
+        <v>These priestesses have been so warped by their channeling of dark powers that they have become insane fanatics, capable of wielding terrifying spells. Requires a Ceyah settlement and a Nightbringer to recruit.</v>
+      </c>
+      <c r="F135" s="1" t="str">
+        <v>Technology Description</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="1" t="n">
+        <v>6142</v>
+      </c>
+      <c r="B136" s="1" t="str">
+        <v>Elite Archer ProperName</v>
+      </c>
+      <c r="C136" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="D136" s="1" t="str">
+        <v>Elite Bowman</v>
+      </c>
+      <c r="E136" s="1" t="str">
+        <v>Elite Bowman</v>
+      </c>
+      <c r="F136" s="1" t="str">
+        <v>Technology ProperName</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="1" t="n">
+        <v>6143</v>
+      </c>
+      <c r="B137" s="1" t="str">
+        <v>Shock Trooper Description</v>
+      </c>
+      <c r="C137" s="1" t="n">
+        <v>173</v>
+      </c>
+      <c r="D137" s="1" t="str">
+        <v>No ground troop is more deadly than the Kohan Elite Guard. Few can stand before them on the field of battle. Requires a Blacksmith, Barracks, Temple, and Library to recruit.</v>
+      </c>
+      <c r="E137" s="1" t="str">
+        <v>No ground troop is more deadly than the Kohan Elite Guard. Few can stand before them on the field of battle. Requires a Blacksmith, Barracks, Temple, and Library to recruit.</v>
+      </c>
+      <c r="F137" s="1" t="str">
+        <v>Technology Description</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="1" t="n">
+        <v>6144</v>
+      </c>
+      <c r="B138" s="1" t="str">
+        <v>Magic Plate Description</v>
+      </c>
+      <c r="C138" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="D138" s="1" t="str">
+        <v>Plate armor constructed with enchanted steel provides more protection than its mundane counterpart.</v>
+      </c>
+      <c r="E138" s="1" t="str">
+        <v>Plate armor constructed with enchanted steel provides more protection than its mundane counterpart.</v>
+      </c>
+      <c r="F138" s="1" t="str">
+        <v>Technology Description</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="1" t="n">
+        <v>6145</v>
+      </c>
+      <c r="B139" s="1" t="str">
+        <v>Bone Reaver Description</v>
+      </c>
+      <c r="C139" s="1" t="n">
+        <v>183</v>
+      </c>
+      <c r="D139" s="1" t="str">
+        <v>Advanced necromantic magicks allow for the creation of more powerful skeletal warriors that move and fight with unholy ferocity. Requires a Ceyah settlement and a Barracks to recruit.</v>
+      </c>
+      <c r="E139" s="1" t="str">
+        <v>Advanced necromantic magicks allow for the creation of more powerful skeletal warriors that move and fight with unholy ferocity. Requires a Ceyah settlement and a Barracks to recruit.</v>
+      </c>
+      <c r="F139" s="1" t="str">
+        <v>Technology Description</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="1" t="n">
+        <v>6146</v>
+      </c>
+      <c r="B140" s="1" t="str">
+        <v>Warlock Description</v>
+      </c>
+      <c r="C140" s="1" t="n">
+        <v>209</v>
+      </c>
+      <c r="D140" s="1" t="str">
+        <v>The enigmatic warlock is privy to strange and powerful magicks that border on the realm of shadow. They first weaken their enemies, then destroy them with torrents of flame. Requires a Mage College to recruit.</v>
+      </c>
+      <c r="E140" s="1" t="str">
+        <v>The enigmatic warlock is privy to strange and powerful magicks that border on the realm of shadow. They first weaken their enemies, then destroy them with torrents of flame. Requires a Mage College to recruit.</v>
+      </c>
+      <c r="F140" s="1" t="str">
+        <v>Technology Description</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="1" t="n">
+        <v>6147</v>
+      </c>
+      <c r="B141" s="1" t="str">
+        <v>Shadowsteel Armor Description</v>
+      </c>
+      <c r="C141" s="1" t="n">
+        <v>163</v>
+      </c>
+      <c r="D141" s="1" t="str">
+        <v>This black chainmail is forged from Shadowsteel. This reduces the weight of the armor without sacrificing protection, allowing warriors to move faster than normal.</v>
+      </c>
+      <c r="E141" s="1" t="str">
+        <v>This black chainmail is forged from Shadowsteel. This reduces the weight of the armor without sacrificing protection, allowing warriors to move faster than normal.</v>
+      </c>
+      <c r="F141" s="1" t="str">
+        <v>Technology Description</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="1" t="n">
+        <v>6148</v>
+      </c>
+      <c r="B142" s="1" t="str">
+        <v>Shadowskin Armor Description</v>
+      </c>
+      <c r="C142" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="D142" s="1" t="str">
+        <v>This leather armor is tainted by the realm of the shadow, making it resistant to non-magical attacks.</v>
+      </c>
+      <c r="E142" s="1" t="str">
+        <v>This leather armor is tainted by the realm of the shadow, making it resistant to non-magical attacks.</v>
+      </c>
+      <c r="F142" s="1" t="str">
+        <v>Technology Description</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="1" t="n">
+        <v>6149</v>
+      </c>
+      <c r="B143" s="1" t="str">
+        <v>Geomancy Description</v>
+      </c>
+      <c r="C143" s="1" t="n">
+        <v>180</v>
+      </c>
+      <c r="D143" s="1" t="str">
+        <v>The elemental magic of geomancy allows the creation of stronger, magically fused stones to be used in the construction of settlements. This increases settlement base health by 35%.</v>
+      </c>
+      <c r="E143" s="1" t="str">
+        <v>The elemental magic of geomancy allows the creation of stronger, magically fused stones to be used in the construction of settlements. This increases settlement base health by 35%.</v>
+      </c>
+      <c r="F143" s="1" t="str">
+        <v>Technology Description</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="1" t="n">
+        <v>6150</v>
+      </c>
+      <c r="B144" s="1" t="str">
+        <v>UnitData ProperName</v>
+      </c>
+      <c r="C144" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="D144" s="1" t="str">
+        <v>Zerin Mordecai</v>
+      </c>
+      <c r="E144" s="1" t="str">
+        <v>Zerin Mordecai</v>
+      </c>
+      <c r="F144" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="1" t="n">
+        <v>6151</v>
+      </c>
+      <c r="B145" s="1" t="str">
+        <v>UnitData ProperName</v>
+      </c>
+      <c r="C145" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="D145" s="1" t="str">
+        <v>Ishan'ghul</v>
+      </c>
+      <c r="E145" s="1" t="str">
+        <v>Ishan'ghul</v>
+      </c>
+      <c r="F145" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="1" t="n">
+        <v>6152</v>
+      </c>
+      <c r="B146" s="1" t="str">
+        <v>UPGRADE_BONUS_MILITIA_MAX Description1</v>
+      </c>
+      <c r="C146" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="D146" s="1" t="str">
+        <v>Increases the maximum number of militia to %d%% of normal.</v>
+      </c>
+      <c r="E146" s="1" t="str">
+        <v>Increases the maximum number of militia to %d%% of normal.</v>
+      </c>
+      <c r="F146" s="1" t="str">
+        <v>Militia Maximum Bonus Description</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="1" t="n">
+        <v>6153</v>
+      </c>
+      <c r="B147" s="1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C147" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="D147" s="1" t="str">
+        <v>The black magicks of this spell temporarily turn the caster into a ghostly shade, immaterial, and resistant to the weapons of mortals.</v>
+      </c>
+      <c r="E147" s="1" t="str">
+        <v>The black magicks of this spell temporarily turn the caster into a ghostly shade, immaterial, and resistant to the weapons of mortals.</v>
+      </c>
+      <c r="F147" s="1" t="str">
+        <v>Spectral Form spell description</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="1" t="n">
+        <v>6154</v>
+      </c>
+      <c r="B148" s="1" t="str">
+        <v>Slaanri Auxiliaries ProperName</v>
+      </c>
+      <c r="C148" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="D148" s="1" t="str">
+        <v>Slaanri Auxiliaries</v>
+      </c>
+      <c r="E148" s="1" t="str">
+        <v>Slaanri Auxiliaries</v>
+      </c>
+      <c r="F148" s="1" t="str">
+        <v>Technology ProperName</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="1" t="n">
+        <v>6155</v>
+      </c>
+      <c r="B149" s="1" t="str">
+        <v>Slaanri Auxiliaries Description</v>
+      </c>
+      <c r="C149" s="1" t="n">
+        <v>314</v>
+      </c>
+      <c r="D149" s="1" t="str">
+        <v>The Slaanri Champions are the strongest and deadliest of the Slaanri warriors. In honor of their powerful and violent cousins, they wield forked bone spears in combat. They have taught the construction technique of these fearsome weapons, allowing for the creation of more effective arms for spear wielding troops.</v>
+      </c>
+      <c r="E149" s="1" t="str">
+        <v>The Slaanri Champions are the strongest and deadliest of the Slaanri warriors. In honor of their powerful and violent cousins, they wield forked bone spears in combat. They have taught the construction technique of these fearsome weapons, allowing for the creation of more effective arms for spear wielding troops.</v>
+      </c>
+      <c r="F149" s="1" t="str">
+        <v>Technology Description</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="1" t="n">
+        <v>6156</v>
+      </c>
+      <c r="B150" s="1" t="str">
+        <v>Siege Tactics ProperName</v>
+      </c>
+      <c r="C150" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="D150" s="1" t="str">
+        <v>Siege Tactics</v>
+      </c>
+      <c r="E150" s="1" t="str">
+        <v>Siege Tactics</v>
+      </c>
+      <c r="F150" s="1" t="str">
+        <v>Technology ProperName</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="1" t="n">
+        <v>6157</v>
+      </c>
+      <c r="B151" s="1" t="str">
+        <v>Siege Tactics Description</v>
+      </c>
+      <c r="C151" s="1" t="n">
+        <v>173</v>
+      </c>
+      <c r="D151" s="1" t="str">
+        <v>Siege tactics are tactical plans for the construction and use of improvised battlefield fortifications. This increases the speed at which all companies entrench and fortify.</v>
+      </c>
+      <c r="E151" s="1" t="str">
+        <v>Siege tactics are tactical plans for the construction and use of improvised battlefield fortifications. This increases the speed at which all companies entrench and fortify.</v>
+      </c>
+      <c r="F151" s="1" t="str">
+        <v>Technology Description</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="1" t="n">
+        <v>6158</v>
+      </c>
+      <c r="B152" s="1" t="str">
+        <v>Golemancy ProperName</v>
+      </c>
+      <c r="C152" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="D152" s="1" t="str">
+        <v>Golemancy</v>
+      </c>
+      <c r="E152" s="1" t="str">
+        <v>Golemancy</v>
+      </c>
+      <c r="F152" s="1" t="str">
+        <v>Technology ProperName</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="1" t="n">
+        <v>6159</v>
+      </c>
+      <c r="B153" s="1" t="str">
+        <v>Golemancy Description</v>
+      </c>
+      <c r="C153" s="1" t="n">
+        <v>205</v>
+      </c>
+      <c r="D153" s="1" t="str">
+        <v>The use of powerful elemental magic has imbued a semblance of life into the very earth, creating mindless warriors that feel no pain. Those wrought from khaldunite-bearing stone are particularly dangerous.</v>
+      </c>
+      <c r="E153" s="1" t="str">
+        <v>The use of powerful elemental magic has imbued a semblance of life into the very earth, creating mindless warriors that feel no pain. Those wrought from khaldunite-bearing stone are particularly dangerous.</v>
+      </c>
+      <c r="F153" s="1" t="str">
+        <v>Technology Description</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="1" t="n">
+        <v>6160</v>
+      </c>
+      <c r="B154" s="1" t="str">
+        <v>Conjurors' Academy ProperName</v>
+      </c>
+      <c r="C154" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="D154" s="1" t="str">
+        <v>Conjurors' Academy</v>
+      </c>
+      <c r="E154" s="1" t="str">
+        <v>Conjurors' Academy</v>
+      </c>
+      <c r="F154" s="1" t="str">
+        <v>Technology ProperName</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="1" t="n">
+        <v>6161</v>
+      </c>
+      <c r="B155" s="1" t="str">
+        <v>Conjurors' Academy Description</v>
+      </c>
+      <c r="C155" s="1" t="n">
+        <v>331</v>
+      </c>
+      <c r="D155" s="1" t="str">
+        <v>Your kingdom's mages have delved into the dark side of summoning, and these fearsome Conjurors have learned the secret of calling forth creatures of Shadow. Their arcane research has led to new techniques that produce stronger and healthier mystical beasts; All summoned creatures have more health and deal more damage than normal.</v>
+      </c>
+      <c r="E155" s="1" t="str">
+        <v>Your kingdom's mages have delved into the dark side of summoning, and these fearsome Conjurors have learned the secret of calling forth creatures of Shadow. Their arcane research has led to new techniques that produce stronger and healthier mystical beasts; All summoned creatures have more health and deal more damage than normal.</v>
+      </c>
+      <c r="F155" s="1" t="str">
+        <v>Technology Description</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="1" t="n">
+        <v>6162</v>
+      </c>
+      <c r="B156" s="1" t="str">
+        <v>Journeymen Description</v>
+      </c>
+      <c r="C156" s="1" t="n">
+        <v>318</v>
+      </c>
+      <c r="D156" s="1" t="str">
+        <v>The Journeymen's Guild is a special organization of laborers that train craftsmen and masons. Having their guild in your kingdom reduces the costs of constructing new building components and provides highly skilled workers for the construction of new settlements. Journeymen can be recruited in any Mareten settlement.</v>
+      </c>
+      <c r="E156" s="1" t="str">
+        <v>The Journeymen's Guild is a special organization of laborers that train craftsmen and masons. Having their guild in your kingdom reduces the costs of constructing new building components and provides highly skilled workers for the construction of new settlements. Journeymen can be recruited in any Mareten settlement.</v>
+      </c>
+      <c r="F156" s="1" t="str">
+        <v>Technology Description</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="1" t="n">
+        <v>6163</v>
+      </c>
+      <c r="B157" s="1" t="str">
+        <v>ObjectData ProperName</v>
+      </c>
+      <c r="C157" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="D157" s="1" t="str">
+        <v>Journeyman</v>
+      </c>
+      <c r="E157" s="1" t="str">
+        <v>Journeyman</v>
+      </c>
+      <c r="F157" s="1" t="str">
+        <v>PIONEER.INI ProperName</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="1" t="n">
+        <v>6164</v>
+      </c>
+      <c r="B158" s="1" t="str">
+        <v>UnitData Description</v>
+      </c>
+      <c r="C158" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="D158" s="1" t="str">
+        <v>Journeymen are expert craftsmen and builders. They can construct new settlements 50% faster than the less well-trained Settlers.</v>
+      </c>
+      <c r="E158" s="1" t="str">
+        <v>Journeymen are expert craftsmen and builders. They can construct new settlements 50% faster than the less well-trained Settlers.</v>
+      </c>
+      <c r="F158" s="1" t="str">
+        <v>PIONEER.INI Description</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="1" t="n">
+        <v>6165</v>
+      </c>
+      <c r="B159" s="1" t="str">
+        <v>Mercenary Description</v>
+      </c>
+      <c r="C159" s="1" t="n">
+        <v>170</v>
+      </c>
+      <c r="D159" s="1" t="str">
+        <v>The Mercenary is a fast and deadly rogue infantryman who works for the highest bidder. Mercenaries generally use inferior armor and weapons. Requires a Bazaar to recruit.</v>
+      </c>
+      <c r="E159" s="1" t="str">
+        <v>The Mercenary is a fast and deadly rogue infantryman who works for the highest bidder. Mercenaries generally use inferior armor and weapons. Requires a Bazaar to recruit.</v>
+      </c>
+      <c r="F159" s="1" t="str">
+        <v>Technology Description</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="1" t="n">
+        <v>6166</v>
+      </c>
+      <c r="B160" s="1" t="str">
+        <v>Cavalry Tactics Description</v>
+      </c>
+      <c r="C160" s="1" t="n">
+        <v>118</v>
+      </c>
+      <c r="D160" s="1" t="str">
+        <v>Cavalry tactics are expert techniques developed to increase the ability of all mounted troops to combat enemy cavalry.</v>
+      </c>
+      <c r="E160" s="1" t="str">
+        <v>Cavalry tactics are expert techniques developed to increase the ability of all mounted troops to combat enemy cavalry.</v>
+      </c>
+      <c r="F160" s="1" t="str">
+        <v>Technology Description</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="1" t="n">
+        <v>6167</v>
+      </c>
+      <c r="B161" s="1" t="str">
+        <v>Defensive Tactics Description</v>
+      </c>
+      <c r="C161" s="1" t="n">
+        <v>167</v>
+      </c>
+      <c r="D161" s="1" t="str">
+        <v>Defensive tactics are tactical plans developed to increase the defensive positioning of troops during battle. This increases the defense of most trained foot soldiers.</v>
+      </c>
+      <c r="E161" s="1" t="str">
+        <v>Defensive tactics are tactical plans developed to increase the defensive positioning of troops during battle. This increases the defense of most trained foot soldiers.</v>
+      </c>
+      <c r="F161" s="1" t="str">
+        <v>Technology Description</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="1" t="n">
+        <v>6168</v>
+      </c>
+      <c r="B162" s="1" t="str">
+        <v>Combat Tactics Description</v>
+      </c>
+      <c r="C162" s="1" t="n">
+        <v>155</v>
+      </c>
+      <c r="D162" s="1" t="str">
+        <v>Combat tactics are tactical plans developed to maximize combat maneuvers and effectiveness. This increases the combat values of most trained foot soldiers.</v>
+      </c>
+      <c r="E162" s="1" t="str">
+        <v>Combat tactics are tactical plans developed to maximize combat maneuvers and effectiveness. This increases the combat values of most trained foot soldiers.</v>
+      </c>
+      <c r="F162" s="1" t="str">
+        <v>Technology Description</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="1" t="n">
+        <v>6169</v>
+      </c>
+      <c r="B163" s="1" t="str">
+        <v>Maecyne Arrow ProperName</v>
+      </c>
+      <c r="C163" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="D163" s="1" t="str">
+        <v>Maecyne Arrow</v>
+      </c>
+      <c r="E163" s="1" t="str">
+        <v>Maecyne Arrow</v>
+      </c>
+      <c r="F163" s="1" t="str">
+        <v>Technology ProperName</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="1" t="n">
+        <v>6170</v>
+      </c>
+      <c r="B164" s="1" t="str">
+        <v>Crystal Ring Description</v>
+      </c>
+      <c r="C164" s="1" t="n">
+        <v>164</v>
+      </c>
+      <c r="D164" s="1" t="str">
+        <v>Special crystal rings that are capable of amplifying magical power, increasing the melee attacks of casters and harming those that dare strike them in close combat.</v>
+      </c>
+      <c r="E164" s="1" t="str">
+        <v>Special crystal rings that are capable of amplifying magical power, increasing the melee attacks of casters and harming those that dare strike them in close combat.</v>
+      </c>
+      <c r="F164" s="1" t="str">
+        <v>Technology Description</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="1" t="n">
+        <v>6171</v>
+      </c>
+      <c r="B165" s="1" t="str">
+        <v>Silk Armor Description</v>
+      </c>
+      <c r="C165" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="D165" s="1" t="str">
+        <v>Specially crafted spider-silk tunics that are light as air and can be worn under robes that can avert a stray arrow or similar missile with ease.</v>
+      </c>
+      <c r="E165" s="1" t="str">
+        <v>Specially crafted spider-silk tunics that are light as air and can be worn under robes that can avert a stray arrow or similar missile with ease.</v>
+      </c>
+      <c r="F165" s="1" t="str">
+        <v>Technology Description</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="1" t="n">
+        <v>6172</v>
+      </c>
+      <c r="B166" s="1" t="str">
+        <v>Silken Robe Description</v>
+      </c>
+      <c r="C166" s="1" t="n">
+        <v>121</v>
+      </c>
+      <c r="D166" s="1" t="str">
+        <v>Robes woven from the silk of giant spiders, making them lighter and more resistant than the normal mage and priest robes.</v>
+      </c>
+      <c r="E166" s="1" t="str">
+        <v>Robes woven from the silk of giant spiders, making them lighter and more resistant than the normal mage and priest robes.</v>
+      </c>
+      <c r="F166" s="1" t="str">
+        <v>Technology Description</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="1" t="n">
+        <v>6173</v>
+      </c>
+      <c r="B167" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C167" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D167" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E167" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F167" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="1" t="n">
+        <v>6174</v>
+      </c>
+      <c r="B168" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C168" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D168" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E168" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F168" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="1" t="n">
+        <v>6175</v>
+      </c>
+      <c r="B169" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C169" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D169" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E169" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F169" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="1" t="n">
+        <v>6176</v>
+      </c>
+      <c r="B170" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C170" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D170" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E170" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F170" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="1" t="n">
+        <v>6177</v>
+      </c>
+      <c r="B171" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C171" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D171" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E171" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F171" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="1" t="n">
+        <v>6178</v>
+      </c>
+      <c r="B172" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C172" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D172" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E172" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F172" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="1" t="n">
+        <v>6179</v>
+      </c>
+      <c r="B173" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C173" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D173" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E173" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F173" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="1" t="n">
+        <v>6180</v>
+      </c>
+      <c r="B174" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C174" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D174" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E174" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F174" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="1" t="n">
+        <v>6181</v>
+      </c>
+      <c r="B175" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C175" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D175" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E175" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F175" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B176" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C176" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D176" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E176" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F176" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B177" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C177" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D177" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E177" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F177" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B178" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C178" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D178" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E178" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F178" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B179" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C179" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D179" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E179" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F179" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B180" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C180" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D180" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E180" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F180" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B181" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C181" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D181" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E181" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F181" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B182" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C182" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D182" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E182" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F182" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B183" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C183" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D183" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E183" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F183" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B184" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C184" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D184" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E184" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F184" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B185" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C185" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D185" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E185" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F185" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B186" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C186" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D186" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E186" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F186" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B187" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C187" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D187" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E187" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F187" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B188" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C188" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D188" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E188" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F188" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B189" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C189" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D189" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E189" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F189" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B190" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C190" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D190" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E190" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F190" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B191" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C191" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D191" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E191" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F191" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B192" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C192" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D192" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E192" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F192" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B193" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C193" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D193" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E193" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F193" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B194" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C194" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D194" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E194" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F194" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B195" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C195" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D195" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E195" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F195" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B196" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C196" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D196" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E196" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F196" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B197" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C197" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D197" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E197" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F197" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B198" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C198" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D198" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E198" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F198" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B199" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C199" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D199" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E199" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F199" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B200" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C200" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D200" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E200" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F200" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Artisan Guild and Pioneer descriptions updated in strings spreadsheet
</commit_message>
<xml_diff>
--- a/Localizations/STRINGS_10.xlsx
+++ b/Localizations/STRINGS_10.xlsx
@@ -1064,19 +1064,19 @@
     <t xml:space="preserve">Your kingdom's mages have delved into the dark side of summoning, and these fearsome Conjurors have learned the secret of calling forth creatures of Shadow. Their arcane research has led to new techniques that produce stronger and healthier mystical beasts; all summoned creatures have more health and deal more damage than normal.</t>
   </si>
   <si>
-    <t xml:space="preserve">Journeymen Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Journeymen's Guild is a special organization of laborers that train craftsmen and masons. Having their guild in your kingdom reduces the costs of constructing new building components and provides highly skilled workers for the construction of new settlements. Journeymen can be recruited in any Mareten settlement.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Journeyman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PIONEER.INI ProperName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Journeymen are expert craftsmen and builders. They can construct new settlements 50% faster than the less well-trained Settlers.</t>
+    <t xml:space="preserve">Artisan Guilds Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Artisan Guilds are a collective of master craftsmen and masons. Their presence in your kingdom lowers the costs of new construction, tools and training as well as attracting more like-minded individuals to settlements where they operate. Within a Masonry Guild, they can outfit and train capable Pioneers to expand the frontiers of the kingdom.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Artisan Guilds ProperName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Artisan Guilds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pioneers are elite settlers, better trained and equipped to expand the kingdom’s borders. They are intrepid navigators in difficult terrain and take great pride in their work.</t>
   </si>
   <si>
     <t xml:space="preserve">PIONEER.INI Description</t>
@@ -1213,7 +1213,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1242,6 +1242,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1259,17 +1263,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H240"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A151" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D162" activeCellId="0" sqref="D162"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E151" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G159" activeCellId="0" sqref="G159"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.29"/>
@@ -1277,7 +1281,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="68.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="2" width="73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="78.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="78.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4965,7 +4969,7 @@
         <v>STRING_6161_Your_kingdom_s_mages_have_delved_into_the_dark_side_of_summoning__and_these_fearsome_Conjurors_have_learned_the_secret_of_calling_forth_creatures_of_Shadow__Their_arcane_research_has_led_to_new_techniques_that_produce_stronger_and_healthier_mystical_beasts;_all_summoned_creatures_have_more_health_and_deal_more_damage_than_normal_</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="51.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="2" t="n">
         <f aca="false">A155+1</f>
         <v>6162</v>
@@ -4975,51 +4979,51 @@
       </c>
       <c r="C156" s="2" t="n">
         <f aca="false">LEN(D156)</f>
-        <v>318</v>
+        <v>348</v>
       </c>
       <c r="D156" s="2" t="s">
         <v>348</v>
       </c>
       <c r="E156" s="2" t="str">
         <f aca="false">D156</f>
-        <v>The Journeymen's Guild is a special organization of laborers that train craftsmen and masons. Having their guild in your kingdom reduces the costs of constructing new building components and provides highly skilled workers for the construction of new settlements. Journeymen can be recruited in any Mareten settlement.</v>
+        <v>The Artisan Guilds are a collective of master craftsmen and masons. Their presence in your kingdom lowers the costs of new construction, tools and training as well as attracting more like-minded individuals to settlements where they operate. Within a Masonry Guild, they can outfit and train capable Pioneers to expand the frontiers of the kingdom.</v>
       </c>
       <c r="G156" s="1" t="s">
         <v>283</v>
       </c>
       <c r="H156" s="2" t="str">
         <f aca="false">"STRING_"&amp;A156&amp;"_"&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($D156," ","_"),",","_"),".","_"),"'","_"),"-","_"),"%","_"),"+","_")</f>
-        <v>STRING_6162_The_Journeymen_s_Guild_is_a_special_organization_of_laborers_that_train_craftsmen_and_masons__Having_their_guild_in_your_kingdom_reduces_the_costs_of_constructing_new_building_components_and_provides_highly_skilled_workers_for_the_construction_of_new_settlements__Journeymen_can_be_recruited_in_any_Mareten_settlement_</v>
-      </c>
-    </row>
-    <row r="157" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>STRING_6162_The_Artisan_Guilds_are_a_collective_of_master_craftsmen_and_masons__Their_presence_in_your_kingdom_lowers_the_costs_of_new_construction__tools_and_training_as_well_as_attracting_more_like_minded_individuals_to_settlements_where_they_operate__Within_a_Masonry_Guild__they_can_outfit_and_train_capable_Pioneers_to_expand_the_frontiers_of_the_kingdom_</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="2" t="n">
         <f aca="false">A156+1</f>
         <v>6163</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>57</v>
+        <v>349</v>
       </c>
       <c r="C157" s="2" t="n">
         <f aca="false">LEN(D157)</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="E157" s="2" t="str">
         <f aca="false">D157</f>
-        <v>Journeyman</v>
+        <v>Artisan Guilds</v>
       </c>
       <c r="G157" s="1" t="s">
-        <v>350</v>
+        <v>299</v>
       </c>
       <c r="H157" s="2" t="str">
         <f aca="false">"STRING_"&amp;A157&amp;"_"&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($D157," ","_"),",","_"),".","_"),"'","_"),"-","_"),"%","_"),"+","_")</f>
-        <v>STRING_6163_Journeyman</v>
-      </c>
-    </row>
-    <row r="158" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>STRING_6163_Artisan_Guilds</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="2" t="n">
         <f aca="false">A157+1</f>
         <v>6164</v>
@@ -5029,21 +5033,21 @@
       </c>
       <c r="C158" s="2" t="n">
         <f aca="false">LEN(D158)</f>
-        <v>128</v>
-      </c>
-      <c r="D158" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D158" s="7" t="s">
         <v>351</v>
       </c>
       <c r="E158" s="2" t="str">
         <f aca="false">D158</f>
-        <v>Journeymen are expert craftsmen and builders. They can construct new settlements 50% faster than the less well-trained Settlers.</v>
+        <v>Pioneers are elite settlers, better trained and equipped to expand the kingdom’s borders. They are intrepid navigators in difficult terrain and take great pride in their work.</v>
       </c>
       <c r="G158" s="1" t="s">
         <v>352</v>
       </c>
       <c r="H158" s="2" t="str">
         <f aca="false">"STRING_"&amp;A158&amp;"_"&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($D158," ","_"),",","_"),".","_"),"'","_"),"-","_"),"%","_"),"+","_")</f>
-        <v>STRING_6164_Journeymen_are_expert_craftsmen_and_builders__They_can_construct_new_settlements_50__faster_than_the_less_well_trained_Settlers_</v>
+        <v>STRING_6164_Pioneers_are_elite_settlers__better_trained_and_equipped_to_expand_the_kingdom’s_borders__They_are_intrepid_navigators_in_difficult_terrain_and_take_great_pride_in_their_work_</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="39.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5493,8 +5497,8 @@
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5503,22 +5507,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F200"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A142" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A167" activeCellId="0" sqref="A167"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A133" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B156" activeCellId="0" sqref="B156"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.78125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="47.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="27.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="51.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="28.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="28.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8629,16 +8634,16 @@
         <v>6162</v>
       </c>
       <c r="B156" s="1" t="str">
-        <v>Journeymen Description</v>
+        <v>Artisan Guilds Description</v>
       </c>
       <c r="C156" s="1" t="n">
-        <v>318</v>
+        <v>348</v>
       </c>
       <c r="D156" s="1" t="str">
-        <v>The Journeymen's Guild is a special organization of laborers that train craftsmen and masons. Having their guild in your kingdom reduces the costs of constructing new building components and provides highly skilled workers for the construction of new settlements. Journeymen can be recruited in any Mareten settlement.</v>
+        <v>The Artisan Guilds are a collective of master craftsmen and masons. Their presence in your kingdom lowers the costs of new construction, tools and training as well as attracting more like-minded individuals to settlements where they operate. Within a Masonry Guild, they can outfit and train capable Pioneers to expand the frontiers of the kingdom.</v>
       </c>
       <c r="E156" s="1" t="str">
-        <v>The Journeymen's Guild is a special organization of laborers that train craftsmen and masons. Having their guild in your kingdom reduces the costs of constructing new building components and provides highly skilled workers for the construction of new settlements. Journeymen can be recruited in any Mareten settlement.</v>
+        <v>The Artisan Guilds are a collective of master craftsmen and masons. Their presence in your kingdom lowers the costs of new construction, tools and training as well as attracting more like-minded individuals to settlements where they operate. Within a Masonry Guild, they can outfit and train capable Pioneers to expand the frontiers of the kingdom.</v>
       </c>
       <c r="F156" s="1" t="str">
         <v>Technology Description</v>
@@ -8649,19 +8654,19 @@
         <v>6163</v>
       </c>
       <c r="B157" s="1" t="str">
-        <v>ObjectData ProperName</v>
+        <v>Artisan Guilds ProperName</v>
       </c>
       <c r="C157" s="1" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D157" s="1" t="str">
-        <v>Journeyman</v>
+        <v>Artisan Guilds</v>
       </c>
       <c r="E157" s="1" t="str">
-        <v>Journeyman</v>
+        <v>Artisan Guilds</v>
       </c>
       <c r="F157" s="1" t="str">
-        <v>PIONEER.INI ProperName</v>
+        <v>Technology ProperName</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8672,13 +8677,13 @@
         <v>UnitData Description</v>
       </c>
       <c r="C158" s="1" t="n">
-        <v>128</v>
+        <v>175</v>
       </c>
       <c r="D158" s="1" t="str">
-        <v>Journeymen are expert craftsmen and builders. They can construct new settlements 50% faster than the less well-trained Settlers.</v>
+        <v>Pioneers are elite settlers, better trained and equipped to expand the kingdom’s borders. They are intrepid navigators in difficult terrain and take great pride in their work.</v>
       </c>
       <c r="E158" s="1" t="str">
-        <v>Journeymen are expert craftsmen and builders. They can construct new settlements 50% faster than the less well-trained Settlers.</v>
+        <v>Pioneers are elite settlers, better trained and equipped to expand the kingdom’s borders. They are intrepid navigators in difficult terrain and take great pride in their work.</v>
       </c>
       <c r="F158" s="1" t="str">
         <v>PIONEER.INI Description</v>
@@ -9334,7 +9339,7 @@
       <c r="C191" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D191" s="7" t="n">
+      <c r="D191" s="8" t="n">
         <v>0</v>
       </c>
       <c r="E191" s="1" t="n">
@@ -9354,7 +9359,7 @@
       <c r="C192" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D192" s="7" t="n">
+      <c r="D192" s="8" t="n">
         <v>0</v>
       </c>
       <c r="E192" s="1" t="n">
@@ -9374,7 +9379,7 @@
       <c r="C193" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D193" s="7" t="n">
+      <c r="D193" s="8" t="n">
         <v>0</v>
       </c>
       <c r="E193" s="1" t="n">
@@ -9394,7 +9399,7 @@
       <c r="C194" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D194" s="7" t="n">
+      <c r="D194" s="8" t="n">
         <v>0</v>
       </c>
       <c r="E194" s="1" t="n">
@@ -9414,7 +9419,7 @@
       <c r="C195" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D195" s="7" t="n">
+      <c r="D195" s="8" t="n">
         <v>0</v>
       </c>
       <c r="E195" s="1" t="n">
@@ -9434,7 +9439,7 @@
       <c r="C196" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D196" s="7" t="n">
+      <c r="D196" s="8" t="n">
         <v>0</v>
       </c>
       <c r="E196" s="1" t="n">
@@ -9454,7 +9459,7 @@
       <c r="C197" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D197" s="7" t="n">
+      <c r="D197" s="8" t="n">
         <v>0</v>
       </c>
       <c r="E197" s="1" t="n">
@@ -9474,7 +9479,7 @@
       <c r="C198" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D198" s="7" t="n">
+      <c r="D198" s="8" t="n">
         <v>0</v>
       </c>
       <c r="E198" s="1" t="n">
@@ -9494,7 +9499,7 @@
       <c r="C199" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D199" s="7" t="n">
+      <c r="D199" s="8" t="n">
         <v>0</v>
       </c>
       <c r="E199" s="1" t="n">
@@ -9514,7 +9519,7 @@
       <c r="C200" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D200" s="7" t="n">
+      <c r="D200" s="8" t="n">
         <v>0</v>
       </c>
       <c r="E200" s="1" t="n">
@@ -9527,10 +9532,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>